<commit_message>
Escaletas y ajustes de recurso
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/Escaleta_CN_11_02_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion02/Escaleta_CN_11_02_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PLANETA 10 Y 11\CN_11_02_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado11\guion02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -727,7 +727,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -797,6 +797,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -893,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -956,69 +962,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1066,84 +1009,151 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,7 +1214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1239,7 +1249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1451,125 +1461,125 @@
   <dimension ref="A1:U284"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N21" sqref="N21"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="78" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" style="78" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="70.28515625" style="78" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.265625" style="55" customWidth="1"/>
+    <col min="5" max="5" width="34.1328125" style="55" customWidth="1"/>
+    <col min="6" max="6" width="30.1328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="70.265625" style="55" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.73046875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="10" width="110" style="78" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
-    <col min="13" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="122.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="110" style="55" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1328125" customWidth="1"/>
+    <col min="12" max="12" width="17.3984375" customWidth="1"/>
+    <col min="13" max="14" width="9.265625" customWidth="1"/>
+    <col min="15" max="15" width="122.1328125" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="16.3984375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.3984375" style="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.85546875" customWidth="1"/>
+    <col min="19" max="19" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="26" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:21" s="26" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="92" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="92" t="s">
+      <c r="J1" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="K1" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="38" t="s">
+      <c r="L1" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="42"/>
-      <c r="O1" s="32" t="s">
+      <c r="N1" s="89"/>
+      <c r="O1" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="71" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="75" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="T1" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="71" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="39"/>
+    <row r="2" spans="1:21" s="26" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="82"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="97"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="84"/>
       <c r="M2" s="27" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="46"/>
-    </row>
-    <row r="3" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="74"/>
+      <c r="U2" s="72"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A3" s="15" t="s">
         <v>17</v>
       </c>
@@ -1579,12 +1589,12 @@
       <c r="C3" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="82"/>
+      <c r="E3" s="57"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="61" t="s">
         <v>125</v>
       </c>
       <c r="H3" s="18">
@@ -1593,7 +1603,7 @@
       <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="65" t="s">
         <v>126</v>
       </c>
       <c r="K3" s="7" t="s">
@@ -1612,23 +1622,23 @@
       <c r="P3" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="Q3" s="28">
+      <c r="Q3" s="98">
         <v>8</v>
       </c>
-      <c r="R3" s="24" t="s">
+      <c r="R3" s="99" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="23" t="s">
+      <c r="S3" s="99" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="99" t="s">
         <v>132</v>
       </c>
-      <c r="U3" s="23" t="s">
+      <c r="U3" s="99" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="15" t="s">
         <v>17</v>
       </c>
@@ -1638,14 +1648,14 @@
       <c r="C4" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="57" t="s">
         <v>125</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="61" t="s">
         <v>133</v>
       </c>
       <c r="H4" s="18">
@@ -1654,7 +1664,7 @@
       <c r="I4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="94" t="s">
+      <c r="J4" s="65" t="s">
         <v>187</v>
       </c>
       <c r="K4" s="7" t="s">
@@ -1687,7 +1697,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -1697,14 +1707,14 @@
       <c r="C5" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="57" t="s">
         <v>125</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="88" t="s">
+      <c r="G5" s="61" t="s">
         <v>134</v>
       </c>
       <c r="H5" s="18">
@@ -1713,7 +1723,7 @@
       <c r="I5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="94" t="s">
+      <c r="J5" s="65" t="s">
         <v>190</v>
       </c>
       <c r="K5" s="7" t="s">
@@ -1746,66 +1756,66 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
+    <row r="6" spans="1:21" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="89" t="s">
+      <c r="F6" s="33"/>
+      <c r="G6" s="62" t="s">
         <v>188</v>
       </c>
-      <c r="H6" s="56">
+      <c r="H6" s="35">
         <v>4</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="95" t="s">
+      <c r="J6" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="K6" s="57" t="s">
+      <c r="K6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="55" t="s">
+      <c r="L6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58" t="s">
+      <c r="M6" s="37"/>
+      <c r="N6" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54" t="s">
+      <c r="O6" s="33"/>
+      <c r="P6" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="Q6" s="59">
+      <c r="Q6" s="38">
         <v>6</v>
       </c>
-      <c r="R6" s="60" t="s">
+      <c r="R6" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="S6" s="61" t="s">
+      <c r="S6" s="40" t="s">
         <v>136</v>
       </c>
-      <c r="T6" s="62" t="s">
+      <c r="T6" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="U6" s="61" t="s">
+      <c r="U6" s="40" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
@@ -1815,12 +1825,12 @@
       <c r="C7" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="79" t="s">
+      <c r="D7" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="E7" s="84"/>
+      <c r="E7" s="59"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="88" t="s">
+      <c r="G7" s="61" t="s">
         <v>141</v>
       </c>
       <c r="H7" s="18">
@@ -1829,7 +1839,7 @@
       <c r="I7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="94" t="s">
+      <c r="J7" s="65" t="s">
         <v>191</v>
       </c>
       <c r="K7" s="20" t="s">
@@ -1862,7 +1872,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A8" s="15" t="s">
         <v>17</v>
       </c>
@@ -1872,12 +1882,12 @@
       <c r="C8" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="82"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="88" t="s">
+      <c r="G8" s="61" t="s">
         <v>192</v>
       </c>
       <c r="H8" s="18">
@@ -1886,7 +1896,7 @@
       <c r="I8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="94" t="s">
+      <c r="J8" s="65" t="s">
         <v>193</v>
       </c>
       <c r="K8" s="7" t="s">
@@ -1901,23 +1911,23 @@
       <c r="P8" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="Q8" s="28">
+      <c r="Q8" s="98">
         <v>8</v>
       </c>
-      <c r="R8" s="24" t="s">
+      <c r="R8" s="99" t="s">
         <v>146</v>
       </c>
-      <c r="S8" s="23" t="s">
+      <c r="S8" s="99" t="s">
         <v>131</v>
       </c>
-      <c r="T8" s="25" t="s">
+      <c r="T8" s="99" t="s">
         <v>147</v>
       </c>
-      <c r="U8" s="23" t="s">
+      <c r="U8" s="99" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
@@ -1927,12 +1937,12 @@
       <c r="C9" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="E9" s="82"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="9"/>
-      <c r="G9" s="88" t="s">
+      <c r="G9" s="61" t="s">
         <v>148</v>
       </c>
       <c r="H9" s="18">
@@ -1941,7 +1951,7 @@
       <c r="I9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="94" t="s">
+      <c r="J9" s="65" t="s">
         <v>194</v>
       </c>
       <c r="K9" s="7" t="s">
@@ -1974,7 +1984,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
@@ -1984,12 +1994,12 @@
       <c r="C10" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D10" s="74" t="s">
+      <c r="D10" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="82"/>
+      <c r="E10" s="57"/>
       <c r="F10" s="9"/>
-      <c r="G10" s="88" t="s">
+      <c r="G10" s="61" t="s">
         <v>153</v>
       </c>
       <c r="H10" s="18">
@@ -1998,7 +2008,7 @@
       <c r="I10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="94" t="s">
+      <c r="J10" s="65" t="s">
         <v>195</v>
       </c>
       <c r="K10" s="7" t="s">
@@ -2029,66 +2039,66 @@
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="71" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="63" t="s">
+    <row r="11" spans="1:21" s="50" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="83" t="s">
+      <c r="E11" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="90" t="s">
+      <c r="F11" s="33"/>
+      <c r="G11" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="45">
         <v>9</v>
       </c>
-      <c r="I11" s="56" t="s">
+      <c r="I11" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="96" t="s">
+      <c r="J11" s="67" t="s">
         <v>196</v>
       </c>
-      <c r="K11" s="57" t="s">
+      <c r="K11" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="L11" s="55" t="s">
+      <c r="L11" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="58"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="54" t="s">
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="P11" s="54" t="s">
+      <c r="P11" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="Q11" s="67">
+      <c r="Q11" s="46">
         <v>10</v>
       </c>
-      <c r="R11" s="68" t="s">
+      <c r="R11" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="S11" s="69" t="s">
+      <c r="S11" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="T11" s="70" t="s">
+      <c r="T11" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="U11" s="69" t="s">
+      <c r="U11" s="48" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
@@ -2098,12 +2108,12 @@
       <c r="C12" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="79" t="s">
+      <c r="D12" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="E12" s="84"/>
+      <c r="E12" s="59"/>
       <c r="F12" s="22"/>
-      <c r="G12" s="88" t="s">
+      <c r="G12" s="61" t="s">
         <v>160</v>
       </c>
       <c r="H12" s="18">
@@ -2112,7 +2122,7 @@
       <c r="I12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="94" t="s">
+      <c r="J12" s="65" t="s">
         <v>158</v>
       </c>
       <c r="K12" s="20" t="s">
@@ -2145,7 +2155,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A13" s="15" t="s">
         <v>17</v>
       </c>
@@ -2155,12 +2165,12 @@
       <c r="C13" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="74" t="s">
+      <c r="D13" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="E13" s="82"/>
+      <c r="E13" s="57"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="61" t="s">
         <v>162</v>
       </c>
       <c r="H13" s="18">
@@ -2169,7 +2179,7 @@
       <c r="I13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="94" t="s">
+      <c r="J13" s="65" t="s">
         <v>197</v>
       </c>
       <c r="K13" s="7" t="s">
@@ -2202,7 +2212,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A14" s="15" t="s">
         <v>17</v>
       </c>
@@ -2212,12 +2222,12 @@
       <c r="C14" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="82"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="88" t="s">
+      <c r="G14" s="61" t="s">
         <v>161</v>
       </c>
       <c r="H14" s="18">
@@ -2226,7 +2236,7 @@
       <c r="I14" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="94" t="s">
+      <c r="J14" s="65" t="s">
         <v>198</v>
       </c>
       <c r="K14" s="7" t="s">
@@ -2257,7 +2267,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A15" s="15" t="s">
         <v>17</v>
       </c>
@@ -2267,12 +2277,12 @@
       <c r="C15" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="E15" s="82"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="88" t="s">
+      <c r="G15" s="61" t="s">
         <v>164</v>
       </c>
       <c r="H15" s="18">
@@ -2281,7 +2291,7 @@
       <c r="I15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="94" t="s">
+      <c r="J15" s="65" t="s">
         <v>199</v>
       </c>
       <c r="K15" s="7" t="s">
@@ -2312,7 +2322,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
@@ -2322,12 +2332,12 @@
       <c r="C16" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="74" t="s">
+      <c r="D16" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="E16" s="82"/>
+      <c r="E16" s="57"/>
       <c r="F16" s="9"/>
-      <c r="G16" s="88" t="s">
+      <c r="G16" s="61" t="s">
         <v>166</v>
       </c>
       <c r="H16" s="18">
@@ -2336,7 +2346,7 @@
       <c r="I16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="94" t="s">
+      <c r="J16" s="65" t="s">
         <v>201</v>
       </c>
       <c r="K16" s="7" t="s">
@@ -2367,7 +2377,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
@@ -2377,12 +2387,12 @@
       <c r="C17" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="74" t="s">
+      <c r="D17" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="E17" s="82"/>
+      <c r="E17" s="57"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="88" t="s">
+      <c r="G17" s="61" t="s">
         <v>167</v>
       </c>
       <c r="H17" s="18">
@@ -2391,7 +2401,7 @@
       <c r="I17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="94" t="s">
+      <c r="J17" s="65" t="s">
         <v>200</v>
       </c>
       <c r="K17" s="7" t="s">
@@ -2424,66 +2434,66 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="71" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="63" t="s">
+    <row r="18" spans="1:21" s="50" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="B18" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="76" t="s">
+      <c r="D18" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="E18" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="54"/>
-      <c r="G18" s="90" t="s">
+      <c r="F18" s="33"/>
+      <c r="G18" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="H18" s="66">
+      <c r="H18" s="45">
         <v>16</v>
       </c>
-      <c r="I18" s="56" t="s">
+      <c r="I18" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="96" t="s">
+      <c r="J18" s="67" t="s">
         <v>202</v>
       </c>
-      <c r="K18" s="57" t="s">
+      <c r="K18" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="55" t="s">
+      <c r="L18" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58" t="s">
+      <c r="M18" s="37"/>
+      <c r="N18" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54" t="s">
+      <c r="O18" s="33"/>
+      <c r="P18" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="Q18" s="67">
+      <c r="Q18" s="46">
         <v>6</v>
       </c>
-      <c r="R18" s="68" t="s">
+      <c r="R18" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="S18" s="69" t="s">
+      <c r="S18" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="T18" s="70" t="s">
+      <c r="T18" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="U18" s="69" t="s">
+      <c r="U18" s="48" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A19" s="15" t="s">
         <v>17</v>
       </c>
@@ -2493,12 +2503,12 @@
       <c r="C19" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="79" t="s">
+      <c r="D19" s="56" t="s">
         <v>169</v>
       </c>
-      <c r="E19" s="84"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="22"/>
-      <c r="G19" s="88" t="s">
+      <c r="G19" s="61" t="s">
         <v>170</v>
       </c>
       <c r="H19" s="18">
@@ -2507,7 +2517,7 @@
       <c r="I19" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="J19" s="94" t="s">
+      <c r="J19" s="65" t="s">
         <v>203</v>
       </c>
       <c r="K19" s="20" t="s">
@@ -2538,7 +2548,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A20" s="15" t="s">
         <v>17</v>
       </c>
@@ -2548,12 +2558,12 @@
       <c r="C20" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="74" t="s">
+      <c r="D20" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="E20" s="82"/>
+      <c r="E20" s="57"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="88" t="s">
+      <c r="G20" s="61" t="s">
         <v>171</v>
       </c>
       <c r="H20" s="18">
@@ -2562,7 +2572,7 @@
       <c r="I20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="94" t="s">
+      <c r="J20" s="65" t="s">
         <v>204</v>
       </c>
       <c r="K20" s="7" t="s">
@@ -2593,7 +2603,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A21" s="15" t="s">
         <v>17</v>
       </c>
@@ -2603,12 +2613,12 @@
       <c r="C21" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="74" t="s">
+      <c r="D21" s="51" t="s">
         <v>169</v>
       </c>
-      <c r="E21" s="82"/>
+      <c r="E21" s="57"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="88" t="s">
+      <c r="G21" s="61" t="s">
         <v>177</v>
       </c>
       <c r="H21" s="18">
@@ -2617,7 +2627,7 @@
       <c r="I21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="94" t="s">
+      <c r="J21" s="65" t="s">
         <v>205</v>
       </c>
       <c r="K21" s="7" t="s">
@@ -2650,66 +2660,66 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="71" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="63" t="s">
+    <row r="22" spans="1:21" s="50" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="64" t="s">
+      <c r="B22" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="C22" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="76" t="s">
+      <c r="D22" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="E22" s="83" t="s">
+      <c r="E22" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="F22" s="54"/>
-      <c r="G22" s="90" t="s">
+      <c r="F22" s="33"/>
+      <c r="G22" s="63" t="s">
         <v>178</v>
       </c>
-      <c r="H22" s="66">
+      <c r="H22" s="45">
         <v>20</v>
       </c>
-      <c r="I22" s="56" t="s">
+      <c r="I22" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="96" t="s">
+      <c r="J22" s="67" t="s">
         <v>206</v>
       </c>
-      <c r="K22" s="57" t="s">
+      <c r="K22" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="55" t="s">
+      <c r="L22" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58" t="s">
+      <c r="M22" s="37"/>
+      <c r="N22" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="O22" s="54"/>
-      <c r="P22" s="54" t="s">
+      <c r="O22" s="33"/>
+      <c r="P22" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="Q22" s="67">
+      <c r="Q22" s="46">
         <v>6</v>
       </c>
-      <c r="R22" s="68" t="s">
+      <c r="R22" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="S22" s="69" t="s">
+      <c r="S22" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="T22" s="70" t="s">
+      <c r="T22" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="U22" s="69" t="s">
+      <c r="U22" s="48" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A23" s="15" t="s">
         <v>17</v>
       </c>
@@ -2719,12 +2729,12 @@
       <c r="C23" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="74" t="s">
+      <c r="D23" s="51" t="s">
         <v>185</v>
       </c>
-      <c r="E23" s="84"/>
+      <c r="E23" s="59"/>
       <c r="F23" s="22"/>
-      <c r="G23" s="88" t="s">
+      <c r="G23" s="61" t="s">
         <v>181</v>
       </c>
       <c r="H23" s="18">
@@ -2733,7 +2743,7 @@
       <c r="I23" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="94" t="s">
+      <c r="J23" s="65" t="s">
         <v>207</v>
       </c>
       <c r="K23" s="20" t="s">
@@ -2764,62 +2774,62 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="71" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="63" t="s">
+    <row r="24" spans="1:21" s="50" customFormat="1" ht="16.149999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="64" t="s">
+      <c r="B24" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="76" t="s">
+      <c r="D24" s="53" t="s">
         <v>185</v>
       </c>
-      <c r="E24" s="83"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="90" t="s">
+      <c r="E24" s="58"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="63" t="s">
         <v>179</v>
       </c>
-      <c r="H24" s="66">
+      <c r="H24" s="45">
         <v>22</v>
       </c>
-      <c r="I24" s="56" t="s">
+      <c r="I24" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="96" t="s">
+      <c r="J24" s="67" t="s">
         <v>208</v>
       </c>
-      <c r="K24" s="57" t="s">
+      <c r="K24" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="L24" s="55" t="s">
+      <c r="L24" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="54"/>
-      <c r="P24" s="54" t="s">
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="Q24" s="59">
+      <c r="Q24" s="38">
         <v>8</v>
       </c>
-      <c r="R24" s="60" t="s">
+      <c r="R24" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="S24" s="61" t="s">
+      <c r="S24" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="T24" s="62" t="s">
+      <c r="T24" s="41" t="s">
         <v>179</v>
       </c>
-      <c r="U24" s="61" t="s">
+      <c r="U24" s="40" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A25" s="15" t="s">
         <v>17</v>
       </c>
@@ -2829,12 +2839,12 @@
       <c r="C25" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D25" s="74" t="s">
+      <c r="D25" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="E25" s="84"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="22"/>
-      <c r="G25" s="88" t="s">
+      <c r="G25" s="61" t="s">
         <v>10</v>
       </c>
       <c r="H25" s="18">
@@ -2843,7 +2853,7 @@
       <c r="I25" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="94" t="s">
+      <c r="J25" s="65" t="s">
         <v>209</v>
       </c>
       <c r="K25" s="20" t="s">
@@ -2864,7 +2874,7 @@
       <c r="T25" s="25"/>
       <c r="U25" s="23"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A26" s="15" t="s">
         <v>17</v>
       </c>
@@ -2874,12 +2884,12 @@
       <c r="C26" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="E26" s="82"/>
+      <c r="E26" s="57"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="88" t="s">
+      <c r="G26" s="61" t="s">
         <v>183</v>
       </c>
       <c r="H26" s="18">
@@ -2888,7 +2898,7 @@
       <c r="I26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="94" t="s">
+      <c r="J26" s="65" t="s">
         <v>210</v>
       </c>
       <c r="K26" s="7" t="s">
@@ -2921,7 +2931,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A27" s="15" t="s">
         <v>17</v>
       </c>
@@ -2931,12 +2941,12 @@
       <c r="C27" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D27" s="74" t="s">
+      <c r="D27" s="51" t="s">
         <v>186</v>
       </c>
-      <c r="E27" s="82"/>
+      <c r="E27" s="57"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="88" t="s">
+      <c r="G27" s="61" t="s">
         <v>184</v>
       </c>
       <c r="H27" s="18">
@@ -2945,7 +2955,7 @@
       <c r="I27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="94" t="s">
+      <c r="J27" s="65" t="s">
         <v>211</v>
       </c>
       <c r="K27" s="7" t="s">
@@ -2978,17 +2988,17 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A28" s="15"/>
       <c r="B28" s="16"/>
       <c r="C28" s="17"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="82"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="57"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="88"/>
+      <c r="G28" s="61"/>
       <c r="H28" s="18"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="94"/>
+      <c r="J28" s="65"/>
       <c r="K28" s="7"/>
       <c r="L28" s="6"/>
       <c r="M28" s="8"/>
@@ -3001,17 +3011,17 @@
       <c r="T28" s="12"/>
       <c r="U28" s="10"/>
     </row>
-    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A29" s="15"/>
       <c r="B29" s="16"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="82"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="57"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="88"/>
+      <c r="G29" s="61"/>
       <c r="H29" s="18"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="94"/>
+      <c r="J29" s="65"/>
       <c r="K29" s="7"/>
       <c r="L29" s="6"/>
       <c r="M29" s="8"/>
@@ -3024,17 +3034,17 @@
       <c r="T29" s="12"/>
       <c r="U29" s="10"/>
     </row>
-    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A30" s="15"/>
       <c r="B30" s="16"/>
       <c r="C30" s="17"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="82"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="57"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="88"/>
+      <c r="G30" s="61"/>
       <c r="H30" s="18"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="94"/>
+      <c r="J30" s="65"/>
       <c r="K30" s="7"/>
       <c r="L30" s="6"/>
       <c r="M30" s="8"/>
@@ -3047,17 +3057,17 @@
       <c r="T30" s="12"/>
       <c r="U30" s="10"/>
     </row>
-    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A31" s="4"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14"/>
-      <c r="D31" s="77"/>
-      <c r="E31" s="85"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="60"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="91"/>
+      <c r="G31" s="64"/>
       <c r="H31" s="9"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="94"/>
+      <c r="J31" s="65"/>
       <c r="K31" s="7"/>
       <c r="L31" s="6"/>
       <c r="M31" s="8"/>
@@ -3070,17 +3080,17 @@
       <c r="T31" s="12"/>
       <c r="U31" s="10"/>
     </row>
-    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A32" s="4"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
-      <c r="D32" s="77"/>
-      <c r="E32" s="85"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="60"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="91"/>
+      <c r="G32" s="64"/>
       <c r="H32" s="9"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="94"/>
+      <c r="J32" s="65"/>
       <c r="K32" s="7"/>
       <c r="L32" s="6"/>
       <c r="M32" s="8"/>
@@ -3093,17 +3103,17 @@
       <c r="T32" s="12"/>
       <c r="U32" s="10"/>
     </row>
-    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A33" s="4"/>
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="85"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="60"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="91"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="9"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="94"/>
+      <c r="J33" s="65"/>
       <c r="K33" s="7"/>
       <c r="L33" s="6"/>
       <c r="M33" s="8"/>
@@ -3116,17 +3126,17 @@
       <c r="T33" s="12"/>
       <c r="U33" s="10"/>
     </row>
-    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A34" s="4"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="85"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="60"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="91"/>
+      <c r="G34" s="64"/>
       <c r="H34" s="9"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="94"/>
+      <c r="J34" s="65"/>
       <c r="K34" s="7"/>
       <c r="L34" s="6"/>
       <c r="M34" s="8"/>
@@ -3139,17 +3149,17 @@
       <c r="T34" s="12"/>
       <c r="U34" s="10"/>
     </row>
-    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A35" s="4"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14"/>
-      <c r="D35" s="77"/>
-      <c r="E35" s="85"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="60"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="91"/>
+      <c r="G35" s="64"/>
       <c r="H35" s="9"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="94"/>
+      <c r="J35" s="65"/>
       <c r="K35" s="7"/>
       <c r="L35" s="6"/>
       <c r="M35" s="8"/>
@@ -3162,17 +3172,17 @@
       <c r="T35" s="12"/>
       <c r="U35" s="10"/>
     </row>
-    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A36" s="4"/>
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="85"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="60"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="91"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="9"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="94"/>
+      <c r="J36" s="65"/>
       <c r="K36" s="7"/>
       <c r="L36" s="6"/>
       <c r="M36" s="8"/>
@@ -3185,17 +3195,17 @@
       <c r="T36" s="12"/>
       <c r="U36" s="10"/>
     </row>
-    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A37" s="4"/>
       <c r="B37" s="13"/>
       <c r="C37" s="14"/>
-      <c r="D37" s="77"/>
-      <c r="E37" s="85"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="60"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="91"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="9"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="94"/>
+      <c r="J37" s="65"/>
       <c r="K37" s="7"/>
       <c r="L37" s="6"/>
       <c r="M37" s="8"/>
@@ -3208,17 +3218,17 @@
       <c r="T37" s="12"/>
       <c r="U37" s="10"/>
     </row>
-    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A38" s="4"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="85"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="60"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="91"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="9"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="94"/>
+      <c r="J38" s="65"/>
       <c r="K38" s="7"/>
       <c r="L38" s="6"/>
       <c r="M38" s="8"/>
@@ -3231,17 +3241,17 @@
       <c r="T38" s="12"/>
       <c r="U38" s="10"/>
     </row>
-    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A39" s="4"/>
       <c r="B39" s="13"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="77"/>
-      <c r="E39" s="85"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="91"/>
+      <c r="G39" s="64"/>
       <c r="H39" s="9"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="94"/>
+      <c r="J39" s="65"/>
       <c r="K39" s="7"/>
       <c r="L39" s="6"/>
       <c r="M39" s="8"/>
@@ -3254,17 +3264,17 @@
       <c r="T39" s="12"/>
       <c r="U39" s="10"/>
     </row>
-    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A40" s="4"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="77"/>
-      <c r="E40" s="85"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="91"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="9"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="94"/>
+      <c r="J40" s="65"/>
       <c r="K40" s="7"/>
       <c r="L40" s="6"/>
       <c r="M40" s="8"/>
@@ -3277,17 +3287,17 @@
       <c r="T40" s="12"/>
       <c r="U40" s="10"/>
     </row>
-    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A41" s="4"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
-      <c r="D41" s="77"/>
-      <c r="E41" s="85"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="91"/>
+      <c r="G41" s="64"/>
       <c r="H41" s="9"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="94"/>
+      <c r="J41" s="65"/>
       <c r="K41" s="7"/>
       <c r="L41" s="6"/>
       <c r="M41" s="8"/>
@@ -3300,17 +3310,17 @@
       <c r="T41" s="12"/>
       <c r="U41" s="10"/>
     </row>
-    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A42" s="4"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="77"/>
-      <c r="E42" s="85"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="91"/>
+      <c r="G42" s="64"/>
       <c r="H42" s="9"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="94"/>
+      <c r="J42" s="65"/>
       <c r="K42" s="7"/>
       <c r="L42" s="6"/>
       <c r="M42" s="8"/>
@@ -3323,17 +3333,17 @@
       <c r="T42" s="12"/>
       <c r="U42" s="10"/>
     </row>
-    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A43" s="4"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="85"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="91"/>
+      <c r="G43" s="64"/>
       <c r="H43" s="9"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="94"/>
+      <c r="J43" s="65"/>
       <c r="K43" s="7"/>
       <c r="L43" s="6"/>
       <c r="M43" s="8"/>
@@ -3346,17 +3356,17 @@
       <c r="T43" s="12"/>
       <c r="U43" s="10"/>
     </row>
-    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A44" s="4"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
-      <c r="D44" s="77"/>
-      <c r="E44" s="85"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="60"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="91"/>
+      <c r="G44" s="64"/>
       <c r="H44" s="9"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="94"/>
+      <c r="J44" s="65"/>
       <c r="K44" s="7"/>
       <c r="L44" s="6"/>
       <c r="M44" s="8"/>
@@ -3369,17 +3379,17 @@
       <c r="T44" s="12"/>
       <c r="U44" s="10"/>
     </row>
-    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A45" s="4"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
-      <c r="D45" s="77"/>
-      <c r="E45" s="85"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="91"/>
+      <c r="G45" s="64"/>
       <c r="H45" s="9"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="94"/>
+      <c r="J45" s="65"/>
       <c r="K45" s="7"/>
       <c r="L45" s="6"/>
       <c r="M45" s="8"/>
@@ -3392,17 +3402,17 @@
       <c r="T45" s="12"/>
       <c r="U45" s="10"/>
     </row>
-    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A46" s="4"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
-      <c r="D46" s="77"/>
-      <c r="E46" s="85"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="91"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="9"/>
       <c r="I46" s="5"/>
-      <c r="J46" s="94"/>
+      <c r="J46" s="65"/>
       <c r="K46" s="7"/>
       <c r="L46" s="6"/>
       <c r="M46" s="8"/>
@@ -3415,17 +3425,17 @@
       <c r="T46" s="12"/>
       <c r="U46" s="10"/>
     </row>
-    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A47" s="4"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
-      <c r="D47" s="77"/>
-      <c r="E47" s="85"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="9"/>
-      <c r="G47" s="91"/>
+      <c r="G47" s="64"/>
       <c r="H47" s="9"/>
       <c r="I47" s="5"/>
-      <c r="J47" s="94"/>
+      <c r="J47" s="65"/>
       <c r="K47" s="7"/>
       <c r="L47" s="6"/>
       <c r="M47" s="8"/>
@@ -3438,17 +3448,17 @@
       <c r="T47" s="12"/>
       <c r="U47" s="10"/>
     </row>
-    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A48" s="4"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
-      <c r="D48" s="77"/>
-      <c r="E48" s="85"/>
+      <c r="D48" s="54"/>
+      <c r="E48" s="60"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="91"/>
+      <c r="G48" s="64"/>
       <c r="H48" s="9"/>
       <c r="I48" s="5"/>
-      <c r="J48" s="94"/>
+      <c r="J48" s="65"/>
       <c r="K48" s="7"/>
       <c r="L48" s="6"/>
       <c r="M48" s="8"/>
@@ -3461,17 +3471,17 @@
       <c r="T48" s="12"/>
       <c r="U48" s="10"/>
     </row>
-    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A49" s="4"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
-      <c r="D49" s="77"/>
-      <c r="E49" s="85"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="60"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="91"/>
+      <c r="G49" s="64"/>
       <c r="H49" s="9"/>
       <c r="I49" s="5"/>
-      <c r="J49" s="94"/>
+      <c r="J49" s="65"/>
       <c r="K49" s="7"/>
       <c r="L49" s="6"/>
       <c r="M49" s="8"/>
@@ -3484,17 +3494,17 @@
       <c r="T49" s="12"/>
       <c r="U49" s="10"/>
     </row>
-    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A50" s="4"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
-      <c r="D50" s="77"/>
-      <c r="E50" s="85"/>
+      <c r="D50" s="54"/>
+      <c r="E50" s="60"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="91"/>
+      <c r="G50" s="64"/>
       <c r="H50" s="9"/>
       <c r="I50" s="5"/>
-      <c r="J50" s="94"/>
+      <c r="J50" s="65"/>
       <c r="K50" s="7"/>
       <c r="L50" s="6"/>
       <c r="M50" s="8"/>
@@ -3507,17 +3517,17 @@
       <c r="T50" s="12"/>
       <c r="U50" s="10"/>
     </row>
-    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A51" s="4"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
-      <c r="D51" s="77"/>
-      <c r="E51" s="85"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="60"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="91"/>
+      <c r="G51" s="64"/>
       <c r="H51" s="9"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="94"/>
+      <c r="J51" s="65"/>
       <c r="K51" s="7"/>
       <c r="L51" s="6"/>
       <c r="M51" s="8"/>
@@ -3530,17 +3540,17 @@
       <c r="T51" s="12"/>
       <c r="U51" s="10"/>
     </row>
-    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A52" s="4"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
-      <c r="D52" s="77"/>
-      <c r="E52" s="85"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="60"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="91"/>
+      <c r="G52" s="64"/>
       <c r="H52" s="9"/>
       <c r="I52" s="5"/>
-      <c r="J52" s="94"/>
+      <c r="J52" s="65"/>
       <c r="K52" s="7"/>
       <c r="L52" s="6"/>
       <c r="M52" s="8"/>
@@ -3553,17 +3563,17 @@
       <c r="T52" s="12"/>
       <c r="U52" s="10"/>
     </row>
-    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A53" s="4"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
-      <c r="D53" s="77"/>
-      <c r="E53" s="85"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="60"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="91"/>
+      <c r="G53" s="64"/>
       <c r="H53" s="9"/>
       <c r="I53" s="5"/>
-      <c r="J53" s="94"/>
+      <c r="J53" s="65"/>
       <c r="K53" s="7"/>
       <c r="L53" s="6"/>
       <c r="M53" s="8"/>
@@ -3576,17 +3586,17 @@
       <c r="T53" s="12"/>
       <c r="U53" s="10"/>
     </row>
-    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A54" s="4"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
-      <c r="D54" s="77"/>
-      <c r="E54" s="85"/>
+      <c r="D54" s="54"/>
+      <c r="E54" s="60"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="91"/>
+      <c r="G54" s="64"/>
       <c r="H54" s="9"/>
       <c r="I54" s="5"/>
-      <c r="J54" s="94"/>
+      <c r="J54" s="65"/>
       <c r="K54" s="7"/>
       <c r="L54" s="6"/>
       <c r="M54" s="8"/>
@@ -3599,17 +3609,17 @@
       <c r="T54" s="12"/>
       <c r="U54" s="10"/>
     </row>
-    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A55" s="4"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
-      <c r="D55" s="77"/>
-      <c r="E55" s="85"/>
+      <c r="D55" s="54"/>
+      <c r="E55" s="60"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="91"/>
+      <c r="G55" s="64"/>
       <c r="H55" s="9"/>
       <c r="I55" s="5"/>
-      <c r="J55" s="94"/>
+      <c r="J55" s="65"/>
       <c r="K55" s="7"/>
       <c r="L55" s="6"/>
       <c r="M55" s="8"/>
@@ -3622,17 +3632,17 @@
       <c r="T55" s="12"/>
       <c r="U55" s="10"/>
     </row>
-    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A56" s="4"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
-      <c r="D56" s="77"/>
-      <c r="E56" s="85"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="60"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="91"/>
+      <c r="G56" s="64"/>
       <c r="H56" s="9"/>
       <c r="I56" s="5"/>
-      <c r="J56" s="94"/>
+      <c r="J56" s="65"/>
       <c r="K56" s="7"/>
       <c r="L56" s="6"/>
       <c r="M56" s="8"/>
@@ -3645,17 +3655,17 @@
       <c r="T56" s="12"/>
       <c r="U56" s="10"/>
     </row>
-    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A57" s="4"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="85"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="60"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="91"/>
+      <c r="G57" s="64"/>
       <c r="H57" s="9"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="94"/>
+      <c r="J57" s="65"/>
       <c r="K57" s="7"/>
       <c r="L57" s="6"/>
       <c r="M57" s="8"/>
@@ -3668,17 +3678,17 @@
       <c r="T57" s="12"/>
       <c r="U57" s="10"/>
     </row>
-    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A58" s="4"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
-      <c r="D58" s="77"/>
-      <c r="E58" s="85"/>
+      <c r="D58" s="54"/>
+      <c r="E58" s="60"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="91"/>
+      <c r="G58" s="64"/>
       <c r="H58" s="9"/>
       <c r="I58" s="5"/>
-      <c r="J58" s="94"/>
+      <c r="J58" s="65"/>
       <c r="K58" s="7"/>
       <c r="L58" s="6"/>
       <c r="M58" s="8"/>
@@ -3691,17 +3701,17 @@
       <c r="T58" s="12"/>
       <c r="U58" s="10"/>
     </row>
-    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A59" s="4"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="85"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="60"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="91"/>
+      <c r="G59" s="64"/>
       <c r="H59" s="9"/>
       <c r="I59" s="5"/>
-      <c r="J59" s="94"/>
+      <c r="J59" s="65"/>
       <c r="K59" s="7"/>
       <c r="L59" s="6"/>
       <c r="M59" s="8"/>
@@ -3714,17 +3724,17 @@
       <c r="T59" s="12"/>
       <c r="U59" s="10"/>
     </row>
-    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A60" s="4"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
-      <c r="D60" s="77"/>
-      <c r="E60" s="85"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="60"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="91"/>
+      <c r="G60" s="64"/>
       <c r="H60" s="9"/>
       <c r="I60" s="5"/>
-      <c r="J60" s="94"/>
+      <c r="J60" s="65"/>
       <c r="K60" s="7"/>
       <c r="L60" s="6"/>
       <c r="M60" s="8"/>
@@ -3737,17 +3747,17 @@
       <c r="T60" s="12"/>
       <c r="U60" s="10"/>
     </row>
-    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A61" s="4"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="77"/>
-      <c r="E61" s="85"/>
+      <c r="D61" s="54"/>
+      <c r="E61" s="60"/>
       <c r="F61" s="9"/>
-      <c r="G61" s="91"/>
+      <c r="G61" s="64"/>
       <c r="H61" s="9"/>
       <c r="I61" s="5"/>
-      <c r="J61" s="94"/>
+      <c r="J61" s="65"/>
       <c r="K61" s="7"/>
       <c r="L61" s="6"/>
       <c r="M61" s="8"/>
@@ -3760,17 +3770,17 @@
       <c r="T61" s="12"/>
       <c r="U61" s="10"/>
     </row>
-    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A62" s="4"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
-      <c r="D62" s="77"/>
-      <c r="E62" s="85"/>
+      <c r="D62" s="54"/>
+      <c r="E62" s="60"/>
       <c r="F62" s="9"/>
-      <c r="G62" s="91"/>
+      <c r="G62" s="64"/>
       <c r="H62" s="9"/>
       <c r="I62" s="5"/>
-      <c r="J62" s="94"/>
+      <c r="J62" s="65"/>
       <c r="K62" s="7"/>
       <c r="L62" s="6"/>
       <c r="M62" s="8"/>
@@ -3783,17 +3793,17 @@
       <c r="T62" s="12"/>
       <c r="U62" s="10"/>
     </row>
-    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A63" s="4"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14"/>
-      <c r="D63" s="77"/>
-      <c r="E63" s="85"/>
+      <c r="D63" s="54"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="91"/>
+      <c r="G63" s="64"/>
       <c r="H63" s="9"/>
       <c r="I63" s="5"/>
-      <c r="J63" s="94"/>
+      <c r="J63" s="65"/>
       <c r="K63" s="7"/>
       <c r="L63" s="6"/>
       <c r="M63" s="8"/>
@@ -3806,17 +3816,17 @@
       <c r="T63" s="12"/>
       <c r="U63" s="10"/>
     </row>
-    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A64" s="4"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14"/>
-      <c r="D64" s="77"/>
-      <c r="E64" s="85"/>
+      <c r="D64" s="54"/>
+      <c r="E64" s="60"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="91"/>
+      <c r="G64" s="64"/>
       <c r="H64" s="9"/>
       <c r="I64" s="5"/>
-      <c r="J64" s="97"/>
+      <c r="J64" s="68"/>
       <c r="K64" s="7"/>
       <c r="L64" s="6"/>
       <c r="M64" s="8"/>
@@ -3829,17 +3839,17 @@
       <c r="T64" s="12"/>
       <c r="U64" s="10"/>
     </row>
-    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A65" s="4"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14"/>
-      <c r="D65" s="77"/>
-      <c r="E65" s="85"/>
+      <c r="D65" s="54"/>
+      <c r="E65" s="60"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="91"/>
+      <c r="G65" s="64"/>
       <c r="H65" s="9"/>
       <c r="I65" s="5"/>
-      <c r="J65" s="97"/>
+      <c r="J65" s="68"/>
       <c r="K65" s="7"/>
       <c r="L65" s="6"/>
       <c r="M65" s="8"/>
@@ -3852,17 +3862,17 @@
       <c r="T65" s="12"/>
       <c r="U65" s="10"/>
     </row>
-    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A66" s="4"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
-      <c r="D66" s="77"/>
-      <c r="E66" s="85"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="60"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="91"/>
+      <c r="G66" s="64"/>
       <c r="H66" s="9"/>
       <c r="I66" s="5"/>
-      <c r="J66" s="97"/>
+      <c r="J66" s="68"/>
       <c r="K66" s="7"/>
       <c r="L66" s="6"/>
       <c r="M66" s="8"/>
@@ -3875,17 +3885,17 @@
       <c r="T66" s="12"/>
       <c r="U66" s="10"/>
     </row>
-    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A67" s="4"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14"/>
-      <c r="D67" s="77"/>
-      <c r="E67" s="85"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="60"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="91"/>
+      <c r="G67" s="64"/>
       <c r="H67" s="9"/>
       <c r="I67" s="5"/>
-      <c r="J67" s="97"/>
+      <c r="J67" s="68"/>
       <c r="K67" s="7"/>
       <c r="L67" s="6"/>
       <c r="M67" s="8"/>
@@ -3898,17 +3908,17 @@
       <c r="T67" s="12"/>
       <c r="U67" s="10"/>
     </row>
-    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A68" s="4"/>
       <c r="B68" s="13"/>
       <c r="C68" s="14"/>
-      <c r="D68" s="77"/>
-      <c r="E68" s="85"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="60"/>
       <c r="F68" s="9"/>
-      <c r="G68" s="91"/>
+      <c r="G68" s="64"/>
       <c r="H68" s="9"/>
       <c r="I68" s="5"/>
-      <c r="J68" s="97"/>
+      <c r="J68" s="68"/>
       <c r="K68" s="7"/>
       <c r="L68" s="6"/>
       <c r="M68" s="8"/>
@@ -3921,17 +3931,17 @@
       <c r="T68" s="12"/>
       <c r="U68" s="10"/>
     </row>
-    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A69" s="4"/>
       <c r="B69" s="13"/>
       <c r="C69" s="14"/>
-      <c r="D69" s="77"/>
-      <c r="E69" s="85"/>
+      <c r="D69" s="54"/>
+      <c r="E69" s="60"/>
       <c r="F69" s="9"/>
-      <c r="G69" s="91"/>
+      <c r="G69" s="64"/>
       <c r="H69" s="9"/>
       <c r="I69" s="5"/>
-      <c r="J69" s="97"/>
+      <c r="J69" s="68"/>
       <c r="K69" s="7"/>
       <c r="L69" s="6"/>
       <c r="M69" s="8"/>
@@ -3944,17 +3954,17 @@
       <c r="T69" s="12"/>
       <c r="U69" s="10"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A70" s="4"/>
       <c r="B70" s="13"/>
       <c r="C70" s="14"/>
-      <c r="D70" s="77"/>
-      <c r="E70" s="85"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="60"/>
       <c r="F70" s="9"/>
-      <c r="G70" s="91"/>
+      <c r="G70" s="64"/>
       <c r="H70" s="9"/>
       <c r="I70" s="5"/>
-      <c r="J70" s="97"/>
+      <c r="J70" s="68"/>
       <c r="K70" s="7"/>
       <c r="L70" s="6"/>
       <c r="M70" s="8"/>
@@ -3967,378 +3977,372 @@
       <c r="T70" s="12"/>
       <c r="U70" s="10"/>
     </row>
-    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="129" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="130" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="131" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="132" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="133" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="134" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="135" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="136" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="137" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="138" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="139" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="140" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="141" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="142" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="143" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="144" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="145" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="146" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="147" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="148" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="149" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="150" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="151" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="152" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="153" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="154" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="155" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="156" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="157" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="158" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="159" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="160" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="161" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="162" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="163" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="164" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="165" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="166" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="167" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="168" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="169" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="170" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="171" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="172" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="173" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="174" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="175" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="176" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="177" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="178" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="179" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="180" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="181" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="182" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="183" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="184" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="185" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="186" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="187" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="188" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="189" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="190" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="191" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="192" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="193" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="194" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="195" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="196" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="197" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="198" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="199" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="200" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="201" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="202" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="203" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="204" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="205" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="206" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="207" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="208" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="209" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="210" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="211" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="212" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="213" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="214" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="215" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="216" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="217" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="218" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="219" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="220" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="221" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="222" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="223" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="224" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="225" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="226" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="227" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="228" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="229" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="230" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="231" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="232" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="233" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="234" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="235" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="236" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="237" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="238" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="239" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="240" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="241" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="242" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="243" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="244" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="245" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="246" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="247" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="248" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="249" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="250" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="251" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="252" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="253" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="254" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="255" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="256" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="257" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="258" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="259" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="260" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="261" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="262" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="263" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="264" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="265" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="266" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="267" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="268" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="269" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="270" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="271" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="272" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="273" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="274" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="275" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="276" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="277" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="278" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="279" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="280" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="125" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="126" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="127" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="128" spans="1:1" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="129" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="130" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="131" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="132" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="133" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="134" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="135" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="136" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="137" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="138" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="139" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="140" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="141" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="142" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="143" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="144" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="145" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="146" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="147" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="148" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="149" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="150" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="151" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="152" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="153" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="154" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="155" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="156" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="157" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="158" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="159" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="160" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="161" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="162" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="163" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="164" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="165" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="166" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="167" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="168" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="169" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="170" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="171" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="172" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="173" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="174" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="175" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="176" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="177" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="178" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="179" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="180" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="181" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="182" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="183" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="184" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="185" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="186" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="187" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="188" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="189" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="190" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="191" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="192" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="193" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="194" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="195" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="196" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="197" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="198" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="199" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="200" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="201" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="202" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="203" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="204" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="205" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="206" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="207" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="208" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="209" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="210" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="211" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="212" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="213" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="214" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="215" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="216" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="217" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="218" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="219" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="220" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="221" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="222" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="223" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="224" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="225" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="226" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="227" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="228" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="229" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="230" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="231" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="232" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="233" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="234" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="235" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="236" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="237" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="238" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="239" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="240" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="241" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="242" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="243" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="244" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="245" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="246" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="247" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="248" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="249" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="250" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="251" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="252" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="253" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="254" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="255" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="256" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="257" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="258" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="259" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="260" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="261" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="262" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="263" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="264" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="265" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="266" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="267" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="268" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="269" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="270" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="271" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="272" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="273" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="274" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="275" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="276" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="277" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="278" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="279" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="280" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="281" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="282" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="283" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="284" hidden="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <autoFilter ref="A1:U2">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4353,6 +4357,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4406,27 +4416,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.86328125" style="2" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.86328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.3984375" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.86328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.3984375" style="2" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="2"/>
-    <col min="14" max="14" width="24.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="69.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="2"/>
+    <col min="13" max="13" width="11.3984375" style="2"/>
+    <col min="14" max="14" width="24.1328125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="69.86328125" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.3984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -4443,7 +4453,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -4467,7 +4477,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -4486,7 +4496,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -4505,7 +4515,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -4521,7 +4531,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -4538,7 +4548,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -4555,7 +4565,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4570,7 +4580,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -4585,7 +4595,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -4600,7 +4610,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -4615,7 +4625,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -4630,7 +4640,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -4645,7 +4655,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -4660,7 +4670,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -4675,7 +4685,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -4690,7 +4700,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
@@ -4704,7 +4714,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
@@ -4718,7 +4728,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
@@ -4732,7 +4742,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
@@ -4746,7 +4756,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -4761,7 +4771,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -4776,7 +4786,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -4791,7 +4801,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -4806,7 +4816,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -4821,7 +4831,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -4836,7 +4846,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -4851,7 +4861,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -4866,7 +4876,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -4881,7 +4891,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -4896,7 +4906,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -4911,7 +4921,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -4926,7 +4936,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -4941,7 +4951,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -4956,7 +4966,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -4971,7 +4981,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -4986,7 +4996,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -5001,7 +5011,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -5016,7 +5026,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -5031,7 +5041,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -5046,7 +5056,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -5061,7 +5071,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -5076,7 +5086,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -5091,7 +5101,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -5106,7 +5116,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -5121,7 +5131,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -5136,7 +5146,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -5151,7 +5161,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -5166,7 +5176,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -5178,7 +5188,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -5190,7 +5200,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -5203,7 +5213,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -5216,7 +5226,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -5229,7 +5239,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -5242,7 +5252,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -5255,7 +5265,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -5268,7 +5278,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -5281,7 +5291,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -5294,7 +5304,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -5307,7 +5317,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -5320,7 +5330,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -5333,7 +5343,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -5346,7 +5356,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -5359,7 +5369,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -5372,7 +5382,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -5385,7 +5395,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -5398,7 +5408,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -5411,7 +5421,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -5424,7 +5434,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -5437,7 +5447,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -5450,7 +5460,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -5464,7 +5474,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -5478,7 +5488,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -5492,7 +5502,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -5506,7 +5516,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -5520,7 +5530,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5534,7 +5544,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5548,7 +5558,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5562,7 +5572,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5576,7 +5586,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5590,7 +5600,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5604,7 +5614,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5618,7 +5628,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5632,7 +5642,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5646,7 +5656,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5660,7 +5670,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5674,7 +5684,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5688,7 +5698,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5702,7 +5712,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5716,7 +5726,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5730,7 +5740,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5744,7 +5754,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5758,7 +5768,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5772,7 +5782,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5786,7 +5796,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5800,7 +5810,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5814,7 +5824,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5828,7 +5838,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5842,7 +5852,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5856,7 +5866,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5870,7 +5880,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5884,7 +5894,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -5898,7 +5908,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5912,7 +5922,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -5926,7 +5936,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5940,7 +5950,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -5954,7 +5964,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5968,7 +5978,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -5982,7 +5992,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5996,7 +6006,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -6010,7 +6020,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -6024,7 +6034,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -6038,7 +6048,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -6052,7 +6062,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -6066,7 +6076,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -6080,7 +6090,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -6094,7 +6104,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -6108,7 +6118,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -6122,7 +6132,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -6136,7 +6146,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -6150,7 +6160,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -6164,7 +6174,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -6178,7 +6188,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -6192,7 +6202,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -6206,7 +6216,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -6220,7 +6230,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -6234,7 +6244,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -6248,7 +6258,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -6262,7 +6272,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -6276,7 +6286,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -6290,7 +6300,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -6304,7 +6314,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -6318,7 +6328,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>

</xml_diff>

<commit_message>
guión 11_02 y solicitudes graficas
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/Escaleta_CN_11_02_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion02/Escaleta_CN_11_02_CO.xlsx
@@ -9,26 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16605" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$24</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="212">
   <si>
     <t>Asignatura</t>
   </si>
@@ -406,9 +401,6 @@
     <t>Consolidación</t>
   </si>
   <si>
-    <t>La clasificación de las ondas</t>
-  </si>
-  <si>
     <t>Interactivo que permite reconocer el concepto de onda y su clasificación</t>
   </si>
   <si>
@@ -418,284 +410,263 @@
     <t>En este recurso hay que modificarlo ya que se encuentra las propiedades de ls ondas, hay que eliminar esta parte y colocar concepto de onda y terminar de completar el recurso con alguna actividad o investigaión</t>
   </si>
   <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>CN_08_11_CO</t>
+  </si>
+  <si>
+    <t>Comprende las clases de ondas</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>Recursos M</t>
+  </si>
+  <si>
+    <t>Recurso M4A-01</t>
+  </si>
+  <si>
+    <t>RM_01_01_CO</t>
+  </si>
+  <si>
+    <t>Recurso M11A-01</t>
+  </si>
+  <si>
+    <t>Las características de las ondas</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>Recursos F</t>
+  </si>
+  <si>
+    <t>Recurso F10-01</t>
+  </si>
+  <si>
+    <t>RF_01_01_CO</t>
+  </si>
+  <si>
+    <t>Resuelve un crucigrama sobre las ondas</t>
+  </si>
+  <si>
+    <t>FQ</t>
+  </si>
+  <si>
+    <t>Las ondas de luz y sonido</t>
+  </si>
+  <si>
+    <t>FQ_10_09</t>
+  </si>
+  <si>
+    <t>Modificar preguntas que no hablen de la clasificación y las características de las ondas</t>
+  </si>
+  <si>
+    <t>Conoce las ondas</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Refuerza tu aprendizaje: Las características de las ondas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complementar las preguntas y modificar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refuerza tu aprendizaje: Las ondas  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que permite conocer la función de onda y sus parte partes </t>
+  </si>
+  <si>
+    <t>Propiedad de un onda</t>
+  </si>
+  <si>
+    <t>¿Qué fenómenos ondulatorios conoces?</t>
+  </si>
+  <si>
+    <t>La energía de la onda</t>
+  </si>
+  <si>
+    <t>Comprende los terremotos</t>
+  </si>
+  <si>
+    <t>La geosfera</t>
+  </si>
+  <si>
+    <t>CN_07_15</t>
+  </si>
+  <si>
+    <t>El planeta Tierra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los terremotos </t>
+  </si>
+  <si>
+    <t>CN_08_01</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La energía de la onda</t>
+  </si>
+  <si>
+    <t>Competencias: construcción de un sismógrafo</t>
+  </si>
+  <si>
+    <t>La luz y el sonido</t>
+  </si>
+  <si>
+    <t>Competencias: estudio de las ondas longitudinales y transversales</t>
+  </si>
+  <si>
+    <t>CN_08_08</t>
+  </si>
+  <si>
+    <t>Evaluación</t>
+  </si>
+  <si>
+    <t>Banco de actividades: las ondas</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Acividad que permite comprender la clasificación de las ondas</t>
+  </si>
+  <si>
+    <t>Actividad que permite clasificar las ondas</t>
+  </si>
+  <si>
+    <t>Interactivo que muestra las partes de una onda y sus definiciones</t>
+  </si>
+  <si>
+    <t>Actividad para relacionar los conceptos de las características de las ondas</t>
+  </si>
+  <si>
+    <t>Actividad que permite resolver un crucigrama sobre el tema de las ondas</t>
+  </si>
+  <si>
+    <t>Actividad que permite completar un párrafo sobre el tema de las características de las ondas</t>
+  </si>
+  <si>
+    <t>Actividades sobre las características de las ondas</t>
+  </si>
+  <si>
+    <t>Actividad que permite concer las propiedades o fenómenos de las ondas</t>
+  </si>
+  <si>
+    <t>Actividad que perite recnocer los fenómenos de las ondas en situaciones específicas</t>
+  </si>
+  <si>
+    <t>Actividad que permite conocer cuanto has aprendido con respecto  a los fenómenos ondulatorios</t>
+  </si>
+  <si>
+    <t>Actividades sobre las propiedaes de las ondas</t>
+  </si>
+  <si>
+    <t>Actividad para resolver ejercicios de energía en una onda</t>
+  </si>
+  <si>
+    <t>Actividades sobre la energía de la onda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que permite el estudio de las ondas longitudinales y tranversales </t>
+  </si>
+  <si>
+    <t>Actividad para la construcción de un sismógrafo</t>
+  </si>
+  <si>
+    <t>Mapa conceptual del tema Las ondas</t>
+  </si>
+  <si>
+    <t>Actividad que evalúa los conceptos aprendidos sobre el tema Las ondas</t>
+  </si>
+  <si>
+    <t>Motor que incluye preguntas de respuesta abierta del tema Las ondas</t>
+  </si>
+  <si>
+    <t>m101a</t>
+  </si>
+  <si>
+    <t>Recurso F4-01</t>
+  </si>
+  <si>
+    <t>Recurso M14A-01</t>
+  </si>
+  <si>
+    <t>Recurso M101AP-01</t>
+  </si>
+  <si>
+    <t>m101ap</t>
+  </si>
+  <si>
+    <t>Recurso M101A-03</t>
+  </si>
+  <si>
+    <t>Recurso M101A-02</t>
+  </si>
+  <si>
+    <t>Recurso M4A-02</t>
+  </si>
+  <si>
+    <t>Las ondas: luz y sonido</t>
+  </si>
+  <si>
+    <t>Las clases de ondas y sus propiedades</t>
+  </si>
+  <si>
+    <t>Diferencia las clases de ondas</t>
+  </si>
+  <si>
+    <t>Recuerda conceptos relacionados con las ondas</t>
+  </si>
+  <si>
+    <t>Las ecuaciones de onda</t>
+  </si>
+  <si>
+    <t>Las propiedades de las ondas</t>
+  </si>
+  <si>
+    <t>Los componentes de la ecuación de onda</t>
+  </si>
+  <si>
+    <t>Practica con la ecuación de onda</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las ecuaciones de onda</t>
+  </si>
+  <si>
+    <t>Tipos de ondas y fenómenos ondulatorios</t>
+  </si>
+  <si>
+    <t>La energía de las ondas</t>
+  </si>
+  <si>
+    <t>Potencia e intensidad de las ondas</t>
+  </si>
+  <si>
+    <t>Términos relacionados con la energía de las ondas</t>
+  </si>
+  <si>
+    <t>Interactivo que permite conocer la energía que propaga una onda</t>
+  </si>
+  <si>
+    <t>Actividad que permite conocer los principales conceptos de la potencia e intensidad de las ondas</t>
+  </si>
+  <si>
     <t>si</t>
-  </si>
-  <si>
-    <t>CN</t>
-  </si>
-  <si>
-    <t>CN_08_11_CO</t>
-  </si>
-  <si>
-    <t>Comprende las clases de ondas</t>
-  </si>
-  <si>
-    <t>¿A qué clase de onda pertenece?</t>
-  </si>
-  <si>
-    <t>RM</t>
-  </si>
-  <si>
-    <t>Recursos M</t>
-  </si>
-  <si>
-    <t>Recurso M4A-01</t>
-  </si>
-  <si>
-    <t>RM_01_01_CO</t>
-  </si>
-  <si>
-    <t>Recurso M11A-01</t>
-  </si>
-  <si>
-    <t>Recurso M101A-01</t>
-  </si>
-  <si>
-    <t>Las características de las ondas</t>
-  </si>
-  <si>
-    <t>RF</t>
-  </si>
-  <si>
-    <t>Recursos F</t>
-  </si>
-  <si>
-    <t>Recurso F10-01</t>
-  </si>
-  <si>
-    <t>RF_01_01_CO</t>
-  </si>
-  <si>
-    <t>Resuelve un crucigrama sobre las ondas</t>
-  </si>
-  <si>
-    <t>FQ</t>
-  </si>
-  <si>
-    <t>Las ondas de luz y sonido</t>
-  </si>
-  <si>
-    <t>FQ_10_09</t>
-  </si>
-  <si>
-    <t>Modificar preguntas que no hablen de la clasificación y las características de las ondas</t>
-  </si>
-  <si>
-    <t>Conoce las ondas</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Refuerza tu aprendizaje: Las características de las ondas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complementar las preguntas y modificar </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refuerza tu aprendizaje: Las ondas  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interactivo que permite conocer la función de onda y sus parte partes </t>
-  </si>
-  <si>
-    <t>Propiedad de un onda</t>
-  </si>
-  <si>
-    <t>Las propiedades de la onda</t>
-  </si>
-  <si>
-    <t>la reflexión y refracción de las ondas</t>
-  </si>
-  <si>
-    <t>Descubre la propiedad de la onda</t>
-  </si>
-  <si>
-    <t>La reflexión y la refracción de la luz</t>
-  </si>
-  <si>
-    <t>Aprende en que consiste la refracción</t>
-  </si>
-  <si>
-    <t>Aprende en qué consiste la refracción</t>
-  </si>
-  <si>
-    <t>¿Qué fenómenos ondulatorios conoces?</t>
-  </si>
-  <si>
-    <t>Clasifica según la propiedad de la onda</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Las propiedades de una onda</t>
-  </si>
-  <si>
-    <t>La energía de la onda</t>
-  </si>
-  <si>
-    <t>Los terremotos</t>
-  </si>
-  <si>
-    <t>Comprende los terremotos</t>
-  </si>
-  <si>
-    <t>La geosfera</t>
-  </si>
-  <si>
-    <t>CN_07_15</t>
-  </si>
-  <si>
-    <t>El planeta Tierra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Los terremotos </t>
-  </si>
-  <si>
-    <t>CN_08_01</t>
-  </si>
-  <si>
-    <t>Soluciona problemas de la energía de las ondas</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La energía de la onda</t>
-  </si>
-  <si>
-    <t>Competencias: construcción de un sismógrafo</t>
-  </si>
-  <si>
-    <t>La luz y el sonido</t>
-  </si>
-  <si>
-    <t>Competencias: estudio de las ondas longitudinales y transversales</t>
-  </si>
-  <si>
-    <t>CN_08_08</t>
-  </si>
-  <si>
-    <t>Evaluación</t>
-  </si>
-  <si>
-    <t>Banco de actividades: las ondas</t>
-  </si>
-  <si>
-    <t>Competencias</t>
-  </si>
-  <si>
-    <t>Fin de tema</t>
-  </si>
-  <si>
-    <t>Acividad que permite comprender la clasificación de las ondas</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: Las ondas</t>
-  </si>
-  <si>
-    <t>Actividades sobre las ondas</t>
-  </si>
-  <si>
-    <t>Actividad que permite clasificar las ondas</t>
-  </si>
-  <si>
-    <t>Interactivo que muestra las partes de una onda y sus definiciones</t>
-  </si>
-  <si>
-    <t>recuerda conceptos relacionados con las ondas</t>
-  </si>
-  <si>
-    <t>Actividad para relacionar los conceptos de las características de las ondas</t>
-  </si>
-  <si>
-    <t>Actividad que permite resolver un crucigrama sobre el tema de las ondas</t>
-  </si>
-  <si>
-    <t>Actividad que permite completar un párrafo sobre el tema de las características de las ondas</t>
-  </si>
-  <si>
-    <t>Actividades sobre las características de las ondas</t>
-  </si>
-  <si>
-    <t>Actividad que permite concer las propiedades o fenómenos de las ondas</t>
-  </si>
-  <si>
-    <t>Interactivo que permite conocer la reflexión y la refracción de una onda</t>
-  </si>
-  <si>
-    <t>Actividad para completar el concepo de refacción e la onda</t>
-  </si>
-  <si>
-    <t>Actividad que perite recnocer los fenómenos de las ondas en situaciones específicas</t>
-  </si>
-  <si>
-    <t>Actividad que permite conocer cuanto has aprendido con respecto  a los fenómenos ondulatorios</t>
-  </si>
-  <si>
-    <t>Actividades sobre las propiedaes de las ondas</t>
-  </si>
-  <si>
-    <t>Interactivo que permite conocer qué sucede en enel onterir de la tierra cuando se produce un tterremoto</t>
-  </si>
-  <si>
-    <t>Actividad que permite conocer los principales conceptos de un terremoto</t>
-  </si>
-  <si>
-    <t>Actividad para resolver ejercicios de energía en una onda</t>
-  </si>
-  <si>
-    <t>Actividades sobre la energía de la onda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actividad que permite el estudio de las ondas longitudinales y tranversales </t>
-  </si>
-  <si>
-    <t>Actividad para la construcción de un sismógrafo</t>
-  </si>
-  <si>
-    <t>Mapa conceptual del tema Las ondas</t>
-  </si>
-  <si>
-    <t>Actividad que evalúa los conceptos aprendidos sobre el tema Las ondas</t>
-  </si>
-  <si>
-    <t>Motor que incluye preguntas de respuesta abierta del tema Las ondas</t>
-  </si>
-  <si>
-    <t>m101a</t>
-  </si>
-  <si>
-    <t>Recurso F4-01</t>
-  </si>
-  <si>
-    <t>Recurso M14A-01</t>
-  </si>
-  <si>
-    <t>Recurso M101AP-01</t>
-  </si>
-  <si>
-    <t>m101ap</t>
-  </si>
-  <si>
-    <t>Recurso M101A-03</t>
-  </si>
-  <si>
-    <t>Recurso M101A-02</t>
-  </si>
-  <si>
-    <t>Recurso M4A-02</t>
-  </si>
-  <si>
-    <t>Las ondas: luz y sonido</t>
-  </si>
-  <si>
-    <t>Las clases de ondas y sus propiedades</t>
-  </si>
-  <si>
-    <t>Diferencia las clases de ondas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -722,6 +693,21 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -893,7 +879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -956,15 +942,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -991,9 +968,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1006,9 +980,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1036,9 +1007,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1048,13 +1016,61 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1482,11 +1498,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U121"/>
+  <dimension ref="A1:U118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.4" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1494,13 +1510,13 @@
     <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="29" style="55" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" style="55" customWidth="1"/>
+    <col min="4" max="4" width="29" style="50" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="50" customWidth="1"/>
     <col min="6" max="6" width="3.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="43" style="55" customWidth="1"/>
+    <col min="7" max="7" width="43" style="50" customWidth="1"/>
     <col min="8" max="8" width="5" style="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="110" style="55" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="107.140625" style="50" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" customWidth="1"/>
     <col min="12" max="12" width="17.42578125" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" customWidth="1"/>
@@ -1513,94 +1529,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="26" customFormat="1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="98" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="96" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="79" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="69" t="s">
+      <c r="I1" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="K1" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="77" t="s">
+      <c r="L1" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="83" t="s">
+      <c r="M1" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="83"/>
-      <c r="O1" s="71" t="s">
+      <c r="N1" s="93"/>
+      <c r="O1" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="71" t="s">
+      <c r="P1" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="92" t="s">
+      <c r="Q1" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="96" t="s">
+      <c r="R1" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="92" t="s">
+      <c r="S1" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="94" t="s">
+      <c r="T1" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="92" t="s">
+      <c r="U1" s="102" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="26" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="76"/>
-      <c r="B2" s="74"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="78"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="27" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="72"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="93"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="107"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="105"/>
+      <c r="U2" s="103"/>
     </row>
     <row r="3" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -1612,53 +1628,53 @@
       <c r="C3" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="57"/>
+      <c r="E3" s="52"/>
       <c r="F3" s="9"/>
-      <c r="G3" s="61" t="s">
+      <c r="G3" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="H3" s="63">
+        <v>1</v>
+      </c>
+      <c r="I3" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="18">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="65" t="s">
+      <c r="K3" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="68" t="s">
         <v>57</v>
       </c>
       <c r="N3" s="8"/>
       <c r="O3" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q3" s="28" t="s">
         <v>128</v>
-      </c>
-      <c r="P3" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q3" s="28" t="s">
-        <v>130</v>
       </c>
       <c r="R3" s="24">
         <v>8</v>
       </c>
       <c r="S3" s="23" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="T3" s="25" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="U3" s="23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1671,56 +1687,54 @@
       <c r="C4" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="E4" s="57" t="s">
-        <v>125</v>
-      </c>
+      <c r="E4" s="52"/>
       <c r="F4" s="9"/>
-      <c r="G4" s="61" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="18">
+      <c r="G4" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="63">
         <v>2</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="64" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="K4" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="K4" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="8"/>
+      <c r="M4" s="68"/>
       <c r="N4" s="8" t="s">
         <v>44</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q4" s="10">
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="U4" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="S4" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="T4" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>17</v>
       </c>
@@ -1730,115 +1744,111 @@
       <c r="C5" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="E5" s="57" t="s">
-        <v>125</v>
-      </c>
+      <c r="E5" s="52"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="61" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="18">
+      <c r="G5" s="62" t="s">
+        <v>205</v>
+      </c>
+      <c r="H5" s="63">
         <v>3</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="64" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>187</v>
-      </c>
-      <c r="K5" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K5" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="8"/>
+      <c r="M5" s="68"/>
       <c r="N5" s="8" t="s">
         <v>32</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q5" s="28">
         <v>6</v>
       </c>
       <c r="R5" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="T5" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="U5" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="S5" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="T5" s="25" t="s">
+    </row>
+    <row r="6" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="U5" s="23" t="s">
+      <c r="E6" s="54"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="62" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" s="63">
+        <v>4</v>
+      </c>
+      <c r="I6" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="K6" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="21"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>6</v>
+      </c>
+      <c r="R6" s="24" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="62" t="s">
-        <v>185</v>
-      </c>
-      <c r="H6" s="35">
-        <v>4</v>
-      </c>
-      <c r="I6" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="66" t="s">
-        <v>186</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q6" s="38">
-        <v>6</v>
-      </c>
-      <c r="R6" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="S6" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="T6" s="41" t="s">
+      <c r="S6" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T6" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="U6" s="40" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="23" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>17</v>
       </c>
@@ -1848,51 +1858,49 @@
       <c r="C7" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="56" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="59"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="61" t="s">
-        <v>140</v>
-      </c>
-      <c r="H7" s="18">
+      <c r="D7" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="E7" s="52"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="62" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="63">
         <v>5</v>
       </c>
-      <c r="I7" s="18" t="s">
-        <v>19</v>
+      <c r="I7" s="64" t="s">
+        <v>20</v>
       </c>
       <c r="J7" s="65" t="s">
-        <v>188</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q7" s="28">
-        <v>6</v>
-      </c>
-      <c r="R7" s="24" t="s">
-        <v>141</v>
+        <v>173</v>
+      </c>
+      <c r="K7" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="68"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q7" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="R7" s="24">
+        <v>8</v>
       </c>
       <c r="S7" s="23" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="T7" s="25" t="s">
-        <v>143</v>
+        <v>198</v>
       </c>
       <c r="U7" s="23" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1905,49 +1913,51 @@
       <c r="C8" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="51" t="s">
-        <v>140</v>
-      </c>
-      <c r="E8" s="57"/>
+      <c r="D8" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="E8" s="52"/>
       <c r="F8" s="9"/>
-      <c r="G8" s="61" t="s">
-        <v>189</v>
-      </c>
-      <c r="H8" s="18">
+      <c r="G8" s="62" t="s">
+        <v>141</v>
+      </c>
+      <c r="H8" s="63">
         <v>6</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="64" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="65" t="s">
-        <v>190</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="K8" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="L8" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="M8" s="8"/>
+      <c r="M8" s="68"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="9"/>
+      <c r="O8" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="P8" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q8" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="R8" s="24">
-        <v>8</v>
-      </c>
-      <c r="S8" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="T8" s="25" t="s">
-        <v>219</v>
-      </c>
-      <c r="U8" s="23" t="s">
-        <v>131</v>
+        <v>126</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>10</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="T8" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="U8" s="10" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -1960,168 +1970,168 @@
       <c r="C9" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="52"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="62" t="s">
+        <v>146</v>
+      </c>
+      <c r="H9" s="63">
+        <v>7</v>
+      </c>
+      <c r="I9" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="65" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="L9" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="68"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q9" s="28">
+        <v>10</v>
+      </c>
+      <c r="R9" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="S9" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="T9" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="U9" s="23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="46" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10" s="30"/>
+      <c r="G10" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="H10" s="63">
+        <v>8</v>
+      </c>
+      <c r="I10" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="K10" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="L10" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="77"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="P10" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q10" s="42">
+        <v>10</v>
+      </c>
+      <c r="R10" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="S10" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="T10" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="U10" s="44" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="54"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="62" t="s">
+        <v>200</v>
+      </c>
+      <c r="H11" s="63">
+        <v>9</v>
+      </c>
+      <c r="I11" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="70" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="21"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q11" s="28">
+        <v>6</v>
+      </c>
+      <c r="R11" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="S11" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="T11" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="U11" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="57"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="61" t="s">
-        <v>145</v>
-      </c>
-      <c r="H9" s="18">
-        <v>7</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="P9" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q9" s="10">
-        <v>10</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="T9" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>140</v>
-      </c>
-      <c r="E10" s="57"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="61" t="s">
-        <v>150</v>
-      </c>
-      <c r="H10" s="18">
-        <v>8</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="65" t="s">
-        <v>192</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q10" s="28">
-        <v>10</v>
-      </c>
-      <c r="R10" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="S10" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="T10" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="U10" s="23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" s="50" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="63" t="s">
-        <v>152</v>
-      </c>
-      <c r="H11" s="45">
-        <v>9</v>
-      </c>
-      <c r="I11" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="67" t="s">
-        <v>193</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="L11" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="33" t="s">
-        <v>153</v>
-      </c>
-      <c r="P11" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q11" s="46">
-        <v>10</v>
-      </c>
-      <c r="R11" s="47" t="s">
-        <v>146</v>
-      </c>
-      <c r="S11" s="48" t="s">
-        <v>147</v>
-      </c>
-      <c r="T11" s="49" t="s">
-        <v>154</v>
-      </c>
-      <c r="U11" s="48" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
@@ -2131,51 +2141,51 @@
       <c r="C12" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="56" t="s">
-        <v>156</v>
-      </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="61" t="s">
-        <v>157</v>
-      </c>
-      <c r="H12" s="18">
+      <c r="D12" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="52"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="78" t="s">
+        <v>202</v>
+      </c>
+      <c r="H12" s="63">
         <v>10</v>
       </c>
-      <c r="I12" s="18" t="s">
-        <v>19</v>
+      <c r="I12" s="64" t="s">
+        <v>20</v>
       </c>
       <c r="J12" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="K12" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="K12" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="M12" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="N12" s="21"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q12" s="28">
+      <c r="L12" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="68"/>
+      <c r="N12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q12" s="29">
         <v>6</v>
       </c>
-      <c r="R12" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="S12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="T12" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="U12" s="23" t="s">
-        <v>144</v>
+      <c r="R12" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="U12" s="10" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2188,51 +2198,51 @@
       <c r="C13" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="E13" s="57"/>
+      <c r="D13" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="52"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="61" t="s">
-        <v>159</v>
-      </c>
-      <c r="H13" s="18">
+      <c r="G13" s="62" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" s="63">
         <v>11</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="64" t="s">
         <v>20</v>
       </c>
       <c r="J13" s="65" t="s">
-        <v>194</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="K13" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="L13" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="M13" s="8"/>
+      <c r="M13" s="68"/>
       <c r="N13" s="8" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="9" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="Q13" s="29">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2245,107 +2255,113 @@
       <c r="C14" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D14" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="E14" s="57"/>
+      <c r="D14" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="52"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="61" t="s">
-        <v>158</v>
-      </c>
-      <c r="H14" s="18">
+      <c r="G14" s="78" t="s">
+        <v>201</v>
+      </c>
+      <c r="H14" s="63">
         <v>12</v>
       </c>
-      <c r="I14" s="5" t="s">
-        <v>19</v>
+      <c r="I14" s="64" t="s">
+        <v>20</v>
       </c>
       <c r="J14" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
+        <v>178</v>
+      </c>
+      <c r="K14" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="67" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14" s="68"/>
+      <c r="N14" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="O14" s="9"/>
       <c r="P14" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q14" s="29">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="46" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="E15" s="57"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="61" t="s">
-        <v>161</v>
-      </c>
-      <c r="H15" s="18">
+      <c r="D15" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15" s="30"/>
+      <c r="G15" s="72" t="s">
+        <v>204</v>
+      </c>
+      <c r="H15" s="63">
         <v>13</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="65" t="s">
-        <v>196</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L15" s="6" t="s">
+      <c r="J15" s="74" t="s">
+        <v>180</v>
+      </c>
+      <c r="K15" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q15" s="28">
-        <v>10</v>
-      </c>
-      <c r="R15" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="S15" s="23" t="s">
-        <v>147</v>
-      </c>
-      <c r="T15" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="U15" s="23" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="77"/>
+      <c r="N15" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q15" s="42">
+        <v>6</v>
+      </c>
+      <c r="R15" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="S15" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="T15" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="U15" s="44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>17</v>
       </c>
@@ -2356,48 +2372,50 @@
         <v>123</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="E16" s="57"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="61" t="s">
-        <v>163</v>
+        <v>154</v>
+      </c>
+      <c r="E16" s="54"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="78" t="s">
+        <v>206</v>
       </c>
       <c r="H16" s="18">
         <v>14</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="65" t="s">
-        <v>198</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L16" s="6" t="s">
+      <c r="I16" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="J16" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="K16" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="N16" s="21"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q16" s="23">
         <v>8</v>
       </c>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q16" s="29">
-        <v>10</v>
-      </c>
-      <c r="R16" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="S16" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="T16" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="U16" s="10" t="s">
-        <v>148</v>
+      <c r="R16" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="S16" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="T16" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="U16" s="23" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2410,13 +2428,13 @@
       <c r="C17" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D17" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="E17" s="57"/>
+      <c r="D17" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="52"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="61" t="s">
-        <v>164</v>
+      <c r="G17" s="78" t="s">
+        <v>207</v>
       </c>
       <c r="H17" s="18">
         <v>15</v>
@@ -2424,154 +2442,156 @@
       <c r="I17" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="65" t="s">
-        <v>197</v>
+      <c r="J17" s="59" t="s">
+        <v>210</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="L17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Q17" s="29">
+        <v>8</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="T17" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" s="52"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="H18" s="18">
+        <v>16</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q18" s="29">
         <v>6</v>
       </c>
-      <c r="R17" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="S17" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="T17" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="U17" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" s="50" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="R18" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T18" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="U18" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="46" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="B19" s="40" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C19" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="D18" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="E18" s="58" t="s">
+      <c r="D19" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="63" t="s">
-        <v>165</v>
-      </c>
-      <c r="H18" s="45">
-        <v>16</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="67" t="s">
-        <v>199</v>
-      </c>
-      <c r="K18" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q18" s="46">
-        <v>6</v>
-      </c>
-      <c r="R18" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="S18" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="T18" s="49" t="s">
-        <v>215</v>
-      </c>
-      <c r="U18" s="48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>166</v>
-      </c>
-      <c r="E19" s="59"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="61" t="s">
-        <v>167</v>
+      <c r="F19" s="30"/>
+      <c r="G19" s="57" t="s">
+        <v>161</v>
       </c>
       <c r="H19" s="18">
         <v>17</v>
       </c>
-      <c r="I19" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="65" t="s">
-        <v>200</v>
-      </c>
-      <c r="K19" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q19" s="23">
+      <c r="I19" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19" s="60" t="s">
+        <v>182</v>
+      </c>
+      <c r="K19" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="R19" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="S19" s="23" t="s">
-        <v>171</v>
-      </c>
-      <c r="T19" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="U19" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="34"/>
+      <c r="N19" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q19" s="42">
+        <v>6</v>
+      </c>
+      <c r="R19" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="S19" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="T19" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="U19" s="44" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>17</v>
       </c>
@@ -2581,168 +2601,152 @@
       <c r="C20" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="E20" s="57"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="61" t="s">
+      <c r="D20" s="47" t="s">
         <v>168</v>
+      </c>
+      <c r="E20" s="54"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="56" t="s">
+        <v>164</v>
       </c>
       <c r="H20" s="18">
         <v>18</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I20" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="65" t="s">
-        <v>201</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="L20" s="6" t="s">
+      <c r="J20" s="59" t="s">
+        <v>183</v>
+      </c>
+      <c r="K20" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="L20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q20" s="29">
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q20" s="28">
         <v>8</v>
       </c>
-      <c r="R20" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="T20" s="12" t="s">
+      <c r="R20" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="S20" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="T20" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="U20" s="23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="46" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="U20" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="61" t="s">
-        <v>174</v>
+      <c r="E21" s="53"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="57" t="s">
+        <v>162</v>
       </c>
       <c r="H21" s="18">
         <v>19</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="I21" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="65" t="s">
-        <v>202</v>
-      </c>
-      <c r="K21" s="7" t="s">
+      <c r="J21" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="K21" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="L21" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q21" s="35">
+        <v>8</v>
+      </c>
+      <c r="R21" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="S21" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="T21" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="U21" s="37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="54"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="18">
         <v>20</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q21" s="29">
-        <v>6</v>
-      </c>
-      <c r="R21" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="T21" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="U21" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" s="50" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="53" t="s">
-        <v>166</v>
-      </c>
-      <c r="E22" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="63" t="s">
-        <v>175</v>
-      </c>
-      <c r="H22" s="45">
+      <c r="I22" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I22" s="35" t="s">
+      <c r="J22" s="59" t="s">
+        <v>185</v>
+      </c>
+      <c r="K22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="67" t="s">
-        <v>203</v>
-      </c>
-      <c r="K22" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q22" s="46">
-        <v>6</v>
-      </c>
-      <c r="R22" s="47" t="s">
-        <v>134</v>
-      </c>
-      <c r="S22" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="T22" s="49" t="s">
-        <v>214</v>
-      </c>
-      <c r="U22" s="48" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="23"/>
+    </row>
+    <row r="23" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>17</v>
       </c>
@@ -2752,276 +2756,190 @@
       <c r="C23" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="51" t="s">
-        <v>182</v>
-      </c>
-      <c r="E23" s="59"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="61" t="s">
-        <v>178</v>
+      <c r="D23" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" s="52"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="56" t="s">
+        <v>166</v>
       </c>
       <c r="H23" s="18">
         <v>21</v>
       </c>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="65" t="s">
-        <v>204</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="L23" s="19" t="s">
+      <c r="J23" s="59" t="s">
+        <v>186</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q23" s="28">
+      <c r="M23" s="8"/>
+      <c r="N23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q23" s="29">
+        <v>6</v>
+      </c>
+      <c r="R23" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S23" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T23" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="U23" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="E24" s="52"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="56" t="s">
+        <v>167</v>
+      </c>
+      <c r="H24" s="18">
+        <v>22</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="S23" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="T23" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="U23" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" s="50" customFormat="1" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="43" t="s">
-        <v>122</v>
-      </c>
-      <c r="C24" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="53" t="s">
-        <v>182</v>
-      </c>
-      <c r="E24" s="58"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="H24" s="45">
-        <v>22</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="67" t="s">
-        <v>205</v>
-      </c>
-      <c r="K24" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q24" s="38">
-        <v>8</v>
-      </c>
-      <c r="R24" s="39" t="s">
-        <v>130</v>
-      </c>
-      <c r="S24" s="40" t="s">
-        <v>171</v>
-      </c>
-      <c r="T24" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="U24" s="40" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="15.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D25" s="51" t="s">
-        <v>183</v>
-      </c>
-      <c r="E25" s="59"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" s="18">
-        <v>23</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="65" t="s">
-        <v>206</v>
-      </c>
-      <c r="K25" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="25"/>
-      <c r="U25" s="23"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q24" s="29">
+        <v>6</v>
+      </c>
+      <c r="R24" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S24" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="T24" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="U24" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>183</v>
-      </c>
-      <c r="E26" s="57"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="52"/>
       <c r="F26" s="9"/>
-      <c r="G26" s="61" t="s">
-        <v>180</v>
-      </c>
-      <c r="H26" s="18">
-        <v>24</v>
-      </c>
-      <c r="I26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="65" t="s">
-        <v>207</v>
-      </c>
-      <c r="K26" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G26" s="56"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="6"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="N26" s="8"/>
       <c r="O26" s="9"/>
-      <c r="P26" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q26" s="29">
-        <v>6</v>
-      </c>
-      <c r="R26" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="T26" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="U26" s="10" t="s">
-        <v>137</v>
-      </c>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D27" s="51" t="s">
-        <v>183</v>
-      </c>
-      <c r="E27" s="57"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="52"/>
       <c r="F27" s="9"/>
-      <c r="G27" s="61" t="s">
-        <v>181</v>
-      </c>
-      <c r="H27" s="18">
-        <v>25</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J27" s="65" t="s">
-        <v>208</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="G27" s="56"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="6"/>
       <c r="M27" s="8"/>
-      <c r="N27" s="8" t="s">
-        <v>213</v>
-      </c>
+      <c r="N27" s="8"/>
       <c r="O27" s="9"/>
-      <c r="P27" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q27" s="29">
-        <v>6</v>
-      </c>
-      <c r="R27" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="S27" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="T27" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="U27" s="10" t="s">
-        <v>137</v>
-      </c>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="10"/>
     </row>
     <row r="28" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="57"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="55"/>
       <c r="F28" s="9"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="18"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="9"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="65"/>
+      <c r="J28" s="59"/>
       <c r="K28" s="7"/>
       <c r="L28" s="6"/>
       <c r="M28" s="8"/>
@@ -3035,16 +2953,16 @@
       <c r="U28" s="10"/>
     </row>
     <row r="29" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="57"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="55"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="18"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="9"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="65"/>
+      <c r="J29" s="59"/>
       <c r="K29" s="7"/>
       <c r="L29" s="6"/>
       <c r="M29" s="8"/>
@@ -3058,16 +2976,16 @@
       <c r="U29" s="10"/>
     </row>
     <row r="30" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="57"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="55"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="18"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="65"/>
+      <c r="J30" s="59"/>
       <c r="K30" s="7"/>
       <c r="L30" s="6"/>
       <c r="M30" s="8"/>
@@ -3084,13 +3002,13 @@
       <c r="A31" s="4"/>
       <c r="B31" s="13"/>
       <c r="C31" s="14"/>
-      <c r="D31" s="54"/>
-      <c r="E31" s="60"/>
+      <c r="D31" s="49"/>
+      <c r="E31" s="55"/>
       <c r="F31" s="9"/>
-      <c r="G31" s="64"/>
+      <c r="G31" s="58"/>
       <c r="H31" s="9"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="65"/>
+      <c r="J31" s="59"/>
       <c r="K31" s="7"/>
       <c r="L31" s="6"/>
       <c r="M31" s="8"/>
@@ -3107,13 +3025,13 @@
       <c r="A32" s="4"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="60"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="55"/>
       <c r="F32" s="9"/>
-      <c r="G32" s="64"/>
+      <c r="G32" s="58"/>
       <c r="H32" s="9"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="65"/>
+      <c r="J32" s="59"/>
       <c r="K32" s="7"/>
       <c r="L32" s="6"/>
       <c r="M32" s="8"/>
@@ -3130,13 +3048,13 @@
       <c r="A33" s="4"/>
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="60"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="55"/>
       <c r="F33" s="9"/>
-      <c r="G33" s="64"/>
+      <c r="G33" s="58"/>
       <c r="H33" s="9"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="65"/>
+      <c r="J33" s="59"/>
       <c r="K33" s="7"/>
       <c r="L33" s="6"/>
       <c r="M33" s="8"/>
@@ -3153,13 +3071,13 @@
       <c r="A34" s="4"/>
       <c r="B34" s="13"/>
       <c r="C34" s="14"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="60"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="55"/>
       <c r="F34" s="9"/>
-      <c r="G34" s="64"/>
+      <c r="G34" s="58"/>
       <c r="H34" s="9"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="65"/>
+      <c r="J34" s="59"/>
       <c r="K34" s="7"/>
       <c r="L34" s="6"/>
       <c r="M34" s="8"/>
@@ -3176,13 +3094,13 @@
       <c r="A35" s="4"/>
       <c r="B35" s="13"/>
       <c r="C35" s="14"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="60"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="55"/>
       <c r="F35" s="9"/>
-      <c r="G35" s="64"/>
+      <c r="G35" s="58"/>
       <c r="H35" s="9"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="65"/>
+      <c r="J35" s="59"/>
       <c r="K35" s="7"/>
       <c r="L35" s="6"/>
       <c r="M35" s="8"/>
@@ -3199,13 +3117,13 @@
       <c r="A36" s="4"/>
       <c r="B36" s="13"/>
       <c r="C36" s="14"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="60"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="55"/>
       <c r="F36" s="9"/>
-      <c r="G36" s="64"/>
+      <c r="G36" s="58"/>
       <c r="H36" s="9"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="65"/>
+      <c r="J36" s="59"/>
       <c r="K36" s="7"/>
       <c r="L36" s="6"/>
       <c r="M36" s="8"/>
@@ -3222,13 +3140,13 @@
       <c r="A37" s="4"/>
       <c r="B37" s="13"/>
       <c r="C37" s="14"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="60"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="64"/>
+      <c r="G37" s="58"/>
       <c r="H37" s="9"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="65"/>
+      <c r="J37" s="59"/>
       <c r="K37" s="7"/>
       <c r="L37" s="6"/>
       <c r="M37" s="8"/>
@@ -3245,13 +3163,13 @@
       <c r="A38" s="4"/>
       <c r="B38" s="13"/>
       <c r="C38" s="14"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="60"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="55"/>
       <c r="F38" s="9"/>
-      <c r="G38" s="64"/>
+      <c r="G38" s="58"/>
       <c r="H38" s="9"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="65"/>
+      <c r="J38" s="59"/>
       <c r="K38" s="7"/>
       <c r="L38" s="6"/>
       <c r="M38" s="8"/>
@@ -3268,13 +3186,13 @@
       <c r="A39" s="4"/>
       <c r="B39" s="13"/>
       <c r="C39" s="14"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="60"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="64"/>
+      <c r="G39" s="58"/>
       <c r="H39" s="9"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="65"/>
+      <c r="J39" s="59"/>
       <c r="K39" s="7"/>
       <c r="L39" s="6"/>
       <c r="M39" s="8"/>
@@ -3291,13 +3209,13 @@
       <c r="A40" s="4"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="60"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="55"/>
       <c r="F40" s="9"/>
-      <c r="G40" s="64"/>
+      <c r="G40" s="58"/>
       <c r="H40" s="9"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="65"/>
+      <c r="J40" s="59"/>
       <c r="K40" s="7"/>
       <c r="L40" s="6"/>
       <c r="M40" s="8"/>
@@ -3314,13 +3232,13 @@
       <c r="A41" s="4"/>
       <c r="B41" s="13"/>
       <c r="C41" s="14"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="60"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="55"/>
       <c r="F41" s="9"/>
-      <c r="G41" s="64"/>
+      <c r="G41" s="58"/>
       <c r="H41" s="9"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="65"/>
+      <c r="J41" s="59"/>
       <c r="K41" s="7"/>
       <c r="L41" s="6"/>
       <c r="M41" s="8"/>
@@ -3337,13 +3255,13 @@
       <c r="A42" s="4"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="60"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="55"/>
       <c r="F42" s="9"/>
-      <c r="G42" s="64"/>
+      <c r="G42" s="58"/>
       <c r="H42" s="9"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="65"/>
+      <c r="J42" s="59"/>
       <c r="K42" s="7"/>
       <c r="L42" s="6"/>
       <c r="M42" s="8"/>
@@ -3360,13 +3278,13 @@
       <c r="A43" s="4"/>
       <c r="B43" s="13"/>
       <c r="C43" s="14"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="60"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="55"/>
       <c r="F43" s="9"/>
-      <c r="G43" s="64"/>
+      <c r="G43" s="58"/>
       <c r="H43" s="9"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="65"/>
+      <c r="J43" s="59"/>
       <c r="K43" s="7"/>
       <c r="L43" s="6"/>
       <c r="M43" s="8"/>
@@ -3383,13 +3301,13 @@
       <c r="A44" s="4"/>
       <c r="B44" s="13"/>
       <c r="C44" s="14"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="60"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="55"/>
       <c r="F44" s="9"/>
-      <c r="G44" s="64"/>
+      <c r="G44" s="58"/>
       <c r="H44" s="9"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="65"/>
+      <c r="J44" s="59"/>
       <c r="K44" s="7"/>
       <c r="L44" s="6"/>
       <c r="M44" s="8"/>
@@ -3406,13 +3324,13 @@
       <c r="A45" s="4"/>
       <c r="B45" s="13"/>
       <c r="C45" s="14"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="60"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="55"/>
       <c r="F45" s="9"/>
-      <c r="G45" s="64"/>
+      <c r="G45" s="58"/>
       <c r="H45" s="9"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="65"/>
+      <c r="J45" s="59"/>
       <c r="K45" s="7"/>
       <c r="L45" s="6"/>
       <c r="M45" s="8"/>
@@ -3429,13 +3347,13 @@
       <c r="A46" s="4"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="60"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="55"/>
       <c r="F46" s="9"/>
-      <c r="G46" s="64"/>
+      <c r="G46" s="58"/>
       <c r="H46" s="9"/>
       <c r="I46" s="5"/>
-      <c r="J46" s="65"/>
+      <c r="J46" s="59"/>
       <c r="K46" s="7"/>
       <c r="L46" s="6"/>
       <c r="M46" s="8"/>
@@ -3452,13 +3370,13 @@
       <c r="A47" s="4"/>
       <c r="B47" s="13"/>
       <c r="C47" s="14"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="60"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="55"/>
       <c r="F47" s="9"/>
-      <c r="G47" s="64"/>
+      <c r="G47" s="58"/>
       <c r="H47" s="9"/>
       <c r="I47" s="5"/>
-      <c r="J47" s="65"/>
+      <c r="J47" s="59"/>
       <c r="K47" s="7"/>
       <c r="L47" s="6"/>
       <c r="M47" s="8"/>
@@ -3475,13 +3393,13 @@
       <c r="A48" s="4"/>
       <c r="B48" s="13"/>
       <c r="C48" s="14"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="60"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="55"/>
       <c r="F48" s="9"/>
-      <c r="G48" s="64"/>
+      <c r="G48" s="58"/>
       <c r="H48" s="9"/>
       <c r="I48" s="5"/>
-      <c r="J48" s="65"/>
+      <c r="J48" s="59"/>
       <c r="K48" s="7"/>
       <c r="L48" s="6"/>
       <c r="M48" s="8"/>
@@ -3498,13 +3416,13 @@
       <c r="A49" s="4"/>
       <c r="B49" s="13"/>
       <c r="C49" s="14"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="60"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="55"/>
       <c r="F49" s="9"/>
-      <c r="G49" s="64"/>
+      <c r="G49" s="58"/>
       <c r="H49" s="9"/>
       <c r="I49" s="5"/>
-      <c r="J49" s="65"/>
+      <c r="J49" s="59"/>
       <c r="K49" s="7"/>
       <c r="L49" s="6"/>
       <c r="M49" s="8"/>
@@ -3521,13 +3439,13 @@
       <c r="A50" s="4"/>
       <c r="B50" s="13"/>
       <c r="C50" s="14"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="60"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="55"/>
       <c r="F50" s="9"/>
-      <c r="G50" s="64"/>
+      <c r="G50" s="58"/>
       <c r="H50" s="9"/>
       <c r="I50" s="5"/>
-      <c r="J50" s="65"/>
+      <c r="J50" s="59"/>
       <c r="K50" s="7"/>
       <c r="L50" s="6"/>
       <c r="M50" s="8"/>
@@ -3544,13 +3462,13 @@
       <c r="A51" s="4"/>
       <c r="B51" s="13"/>
       <c r="C51" s="14"/>
-      <c r="D51" s="54"/>
-      <c r="E51" s="60"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="55"/>
       <c r="F51" s="9"/>
-      <c r="G51" s="64"/>
+      <c r="G51" s="58"/>
       <c r="H51" s="9"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="65"/>
+      <c r="J51" s="59"/>
       <c r="K51" s="7"/>
       <c r="L51" s="6"/>
       <c r="M51" s="8"/>
@@ -3567,13 +3485,13 @@
       <c r="A52" s="4"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
-      <c r="D52" s="54"/>
-      <c r="E52" s="60"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="55"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="64"/>
+      <c r="G52" s="58"/>
       <c r="H52" s="9"/>
       <c r="I52" s="5"/>
-      <c r="J52" s="65"/>
+      <c r="J52" s="59"/>
       <c r="K52" s="7"/>
       <c r="L52" s="6"/>
       <c r="M52" s="8"/>
@@ -3590,13 +3508,13 @@
       <c r="A53" s="4"/>
       <c r="B53" s="13"/>
       <c r="C53" s="14"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="60"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="55"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="64"/>
+      <c r="G53" s="58"/>
       <c r="H53" s="9"/>
       <c r="I53" s="5"/>
-      <c r="J53" s="65"/>
+      <c r="J53" s="59"/>
       <c r="K53" s="7"/>
       <c r="L53" s="6"/>
       <c r="M53" s="8"/>
@@ -3613,13 +3531,13 @@
       <c r="A54" s="4"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="60"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="55"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="64"/>
+      <c r="G54" s="58"/>
       <c r="H54" s="9"/>
       <c r="I54" s="5"/>
-      <c r="J54" s="65"/>
+      <c r="J54" s="59"/>
       <c r="K54" s="7"/>
       <c r="L54" s="6"/>
       <c r="M54" s="8"/>
@@ -3636,13 +3554,13 @@
       <c r="A55" s="4"/>
       <c r="B55" s="13"/>
       <c r="C55" s="14"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="60"/>
+      <c r="D55" s="49"/>
+      <c r="E55" s="55"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="64"/>
+      <c r="G55" s="58"/>
       <c r="H55" s="9"/>
       <c r="I55" s="5"/>
-      <c r="J55" s="65"/>
+      <c r="J55" s="59"/>
       <c r="K55" s="7"/>
       <c r="L55" s="6"/>
       <c r="M55" s="8"/>
@@ -3659,13 +3577,13 @@
       <c r="A56" s="4"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
-      <c r="D56" s="54"/>
-      <c r="E56" s="60"/>
+      <c r="D56" s="49"/>
+      <c r="E56" s="55"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="64"/>
+      <c r="G56" s="58"/>
       <c r="H56" s="9"/>
       <c r="I56" s="5"/>
-      <c r="J56" s="65"/>
+      <c r="J56" s="59"/>
       <c r="K56" s="7"/>
       <c r="L56" s="6"/>
       <c r="M56" s="8"/>
@@ -3682,13 +3600,13 @@
       <c r="A57" s="4"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
-      <c r="D57" s="54"/>
-      <c r="E57" s="60"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="55"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="64"/>
+      <c r="G57" s="58"/>
       <c r="H57" s="9"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="65"/>
+      <c r="J57" s="59"/>
       <c r="K57" s="7"/>
       <c r="L57" s="6"/>
       <c r="M57" s="8"/>
@@ -3705,13 +3623,13 @@
       <c r="A58" s="4"/>
       <c r="B58" s="13"/>
       <c r="C58" s="14"/>
-      <c r="D58" s="54"/>
-      <c r="E58" s="60"/>
+      <c r="D58" s="49"/>
+      <c r="E58" s="55"/>
       <c r="F58" s="9"/>
-      <c r="G58" s="64"/>
+      <c r="G58" s="58"/>
       <c r="H58" s="9"/>
       <c r="I58" s="5"/>
-      <c r="J58" s="65"/>
+      <c r="J58" s="59"/>
       <c r="K58" s="7"/>
       <c r="L58" s="6"/>
       <c r="M58" s="8"/>
@@ -3728,13 +3646,13 @@
       <c r="A59" s="4"/>
       <c r="B59" s="13"/>
       <c r="C59" s="14"/>
-      <c r="D59" s="54"/>
-      <c r="E59" s="60"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="55"/>
       <c r="F59" s="9"/>
-      <c r="G59" s="64"/>
+      <c r="G59" s="58"/>
       <c r="H59" s="9"/>
       <c r="I59" s="5"/>
-      <c r="J59" s="65"/>
+      <c r="J59" s="59"/>
       <c r="K59" s="7"/>
       <c r="L59" s="6"/>
       <c r="M59" s="8"/>
@@ -3751,13 +3669,13 @@
       <c r="A60" s="4"/>
       <c r="B60" s="13"/>
       <c r="C60" s="14"/>
-      <c r="D60" s="54"/>
-      <c r="E60" s="60"/>
+      <c r="D60" s="49"/>
+      <c r="E60" s="55"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="64"/>
+      <c r="G60" s="58"/>
       <c r="H60" s="9"/>
       <c r="I60" s="5"/>
-      <c r="J60" s="65"/>
+      <c r="J60" s="59"/>
       <c r="K60" s="7"/>
       <c r="L60" s="6"/>
       <c r="M60" s="8"/>
@@ -3774,13 +3692,13 @@
       <c r="A61" s="4"/>
       <c r="B61" s="13"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="54"/>
-      <c r="E61" s="60"/>
+      <c r="D61" s="49"/>
+      <c r="E61" s="55"/>
       <c r="F61" s="9"/>
-      <c r="G61" s="64"/>
+      <c r="G61" s="58"/>
       <c r="H61" s="9"/>
       <c r="I61" s="5"/>
-      <c r="J61" s="65"/>
+      <c r="J61" s="61"/>
       <c r="K61" s="7"/>
       <c r="L61" s="6"/>
       <c r="M61" s="8"/>
@@ -3797,13 +3715,13 @@
       <c r="A62" s="4"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="60"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="55"/>
       <c r="F62" s="9"/>
-      <c r="G62" s="64"/>
+      <c r="G62" s="58"/>
       <c r="H62" s="9"/>
       <c r="I62" s="5"/>
-      <c r="J62" s="65"/>
+      <c r="J62" s="61"/>
       <c r="K62" s="7"/>
       <c r="L62" s="6"/>
       <c r="M62" s="8"/>
@@ -3820,13 +3738,13 @@
       <c r="A63" s="4"/>
       <c r="B63" s="13"/>
       <c r="C63" s="14"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="60"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="55"/>
       <c r="F63" s="9"/>
-      <c r="G63" s="64"/>
+      <c r="G63" s="58"/>
       <c r="H63" s="9"/>
       <c r="I63" s="5"/>
-      <c r="J63" s="65"/>
+      <c r="J63" s="61"/>
       <c r="K63" s="7"/>
       <c r="L63" s="6"/>
       <c r="M63" s="8"/>
@@ -3843,13 +3761,13 @@
       <c r="A64" s="4"/>
       <c r="B64" s="13"/>
       <c r="C64" s="14"/>
-      <c r="D64" s="54"/>
-      <c r="E64" s="60"/>
+      <c r="D64" s="49"/>
+      <c r="E64" s="55"/>
       <c r="F64" s="9"/>
-      <c r="G64" s="64"/>
+      <c r="G64" s="58"/>
       <c r="H64" s="9"/>
       <c r="I64" s="5"/>
-      <c r="J64" s="68"/>
+      <c r="J64" s="61"/>
       <c r="K64" s="7"/>
       <c r="L64" s="6"/>
       <c r="M64" s="8"/>
@@ -3866,13 +3784,13 @@
       <c r="A65" s="4"/>
       <c r="B65" s="13"/>
       <c r="C65" s="14"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="60"/>
+      <c r="D65" s="49"/>
+      <c r="E65" s="55"/>
       <c r="F65" s="9"/>
-      <c r="G65" s="64"/>
+      <c r="G65" s="58"/>
       <c r="H65" s="9"/>
       <c r="I65" s="5"/>
-      <c r="J65" s="68"/>
+      <c r="J65" s="61"/>
       <c r="K65" s="7"/>
       <c r="L65" s="6"/>
       <c r="M65" s="8"/>
@@ -3889,13 +3807,13 @@
       <c r="A66" s="4"/>
       <c r="B66" s="13"/>
       <c r="C66" s="14"/>
-      <c r="D66" s="54"/>
-      <c r="E66" s="60"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="55"/>
       <c r="F66" s="9"/>
-      <c r="G66" s="64"/>
+      <c r="G66" s="58"/>
       <c r="H66" s="9"/>
       <c r="I66" s="5"/>
-      <c r="J66" s="68"/>
+      <c r="J66" s="61"/>
       <c r="K66" s="7"/>
       <c r="L66" s="6"/>
       <c r="M66" s="8"/>
@@ -3912,13 +3830,13 @@
       <c r="A67" s="4"/>
       <c r="B67" s="13"/>
       <c r="C67" s="14"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="60"/>
+      <c r="D67" s="49"/>
+      <c r="E67" s="55"/>
       <c r="F67" s="9"/>
-      <c r="G67" s="64"/>
+      <c r="G67" s="58"/>
       <c r="H67" s="9"/>
       <c r="I67" s="5"/>
-      <c r="J67" s="68"/>
+      <c r="J67" s="61"/>
       <c r="K67" s="7"/>
       <c r="L67" s="6"/>
       <c r="M67" s="8"/>
@@ -3931,262 +3849,193 @@
       <c r="T67" s="12"/>
       <c r="U67" s="10"/>
     </row>
-    <row r="68" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="60"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="64"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="5"/>
-      <c r="J68" s="68"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="6"/>
-      <c r="M68" s="8"/>
-      <c r="N68" s="8"/>
-      <c r="O68" s="9"/>
-      <c r="P68" s="9"/>
-      <c r="Q68" s="10"/>
-      <c r="R68" s="11"/>
-      <c r="S68" s="10"/>
-      <c r="T68" s="12"/>
-      <c r="U68" s="10"/>
-    </row>
-    <row r="69" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="14"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="60"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="64"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="5"/>
-      <c r="J69" s="68"/>
-      <c r="K69" s="7"/>
-      <c r="L69" s="6"/>
-      <c r="M69" s="8"/>
-      <c r="N69" s="8"/>
-      <c r="O69" s="9"/>
-      <c r="P69" s="9"/>
-      <c r="Q69" s="10"/>
-      <c r="R69" s="11"/>
-      <c r="S69" s="10"/>
-      <c r="T69" s="12"/>
-      <c r="U69" s="10"/>
-    </row>
-    <row r="70" spans="1:21" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="14"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="60"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="64"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="68"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="6"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="9"/>
-      <c r="P70" s="9"/>
-      <c r="Q70" s="10"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="10"/>
-      <c r="T70" s="12"/>
-      <c r="U70" s="10"/>
+    <row r="82" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="85" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U2">
+  <autoFilter ref="A1:U24">
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
@@ -4220,36 +4069,33 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N70</xm:sqref>
+          <xm:sqref>N3:N67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A70</xm:sqref>
+          <xm:sqref>A3:A67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I70 P3:P70 K3:K70</xm:sqref>
+          <xm:sqref>K3:K67 P3:P67 I3:I67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L70</xm:sqref>
+          <xm:sqref>L3:L67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M70</xm:sqref>
+          <xm:sqref>M3:M67</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -6213,10 +6059,5 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>